<commit_message>
add distilation_2 model DOne
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v2.xlsx
+++ b/excel files/propionate_case_study_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54AAD6F5-FE8F-48E7-B367-8B559C68DEAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF62FEC5-EF7B-4EEF-A34D-2E56D66846FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="248">
   <si>
     <t>components</t>
   </si>
@@ -819,6 +819,9 @@
   </si>
   <si>
     <t>fed-batch (FFB, biomass contained in fibers)</t>
+  </si>
+  <si>
+    <t>Distillation_2.json</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1205,12 +1208,9 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3833,7 +3833,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E7:F8 E12:G12 H2:H4 H7:H8 E3:E4 F2:F4">
+  <conditionalFormatting sqref="E3:E4 E7:F8 E12:G12 F2:F4 H2:H4 H7:H8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -4008,10 +4008,10 @@
       <c r="C11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="D11" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="E11" s="45"/>
+      <c r="E11" s="44"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="30" t="s">
@@ -4026,10 +4026,10 @@
       <c r="D12" t="s">
         <v>218</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="44"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="45"/>
+      <c r="A14" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4083,10 +4083,10 @@
       <c r="C2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="44" t="s">
+      <c r="D2" s="43" t="s">
         <v>237</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="50" t="s">
         <v>238</v>
       </c>
       <c r="F2" t="s">
@@ -4158,8 +4158,8 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O16" sqref="O16"/>
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4192,55 +4192,55 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="49" t="s">
+      <c r="F1" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="48" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="I1" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="48" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="49" t="s">
+      <c r="N1" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="O1" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="P1" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="49" t="s">
+      <c r="Q1" s="48" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="48" t="s">
         <v>73</v>
       </c>
       <c r="T1" s="18" t="s">
@@ -4254,56 +4254,56 @@
       <c r="A2" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="45">
         <v>2</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="E2" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="46">
-        <v>0</v>
-      </c>
-      <c r="G2" s="46">
-        <v>0</v>
-      </c>
-      <c r="H2" s="46">
-        <v>0</v>
-      </c>
-      <c r="I2" s="46" t="s">
+      <c r="F2" s="45">
+        <v>0</v>
+      </c>
+      <c r="G2" s="45">
+        <v>0</v>
+      </c>
+      <c r="H2" s="45">
+        <v>0</v>
+      </c>
+      <c r="I2" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="48">
-        <v>0</v>
-      </c>
-      <c r="M2" s="46">
-        <v>0</v>
-      </c>
-      <c r="N2" s="46">
+      <c r="L2" s="47">
+        <v>0</v>
+      </c>
+      <c r="M2" s="45">
+        <v>0</v>
+      </c>
+      <c r="N2" s="45">
         <f xml:space="preserve"> 0.5*0.001</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O2" s="46" t="s">
+      <c r="O2" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P2" s="46" t="s">
+      <c r="P2" s="45" t="s">
         <v>197</v>
       </c>
-      <c r="Q2" s="46" t="s">
+      <c r="Q2" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="R2" s="46">
+      <c r="R2" s="45">
         <v>0</v>
       </c>
       <c r="T2">
@@ -4317,56 +4317,56 @@
       <c r="A3" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="46">
+      <c r="B3" s="45">
         <v>2</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="46">
-        <v>0</v>
-      </c>
-      <c r="G3" s="46">
-        <v>0</v>
-      </c>
-      <c r="H3" s="46">
-        <v>0</v>
-      </c>
-      <c r="I3" s="46" t="s">
+      <c r="F3" s="45">
+        <v>0</v>
+      </c>
+      <c r="G3" s="45">
+        <v>0</v>
+      </c>
+      <c r="H3" s="45">
+        <v>0</v>
+      </c>
+      <c r="I3" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="46">
-        <v>0</v>
-      </c>
-      <c r="M3" s="46">
-        <v>0</v>
-      </c>
-      <c r="N3" s="46">
+      <c r="L3" s="45">
+        <v>0</v>
+      </c>
+      <c r="M3" s="45">
+        <v>0</v>
+      </c>
+      <c r="N3" s="45">
         <f t="shared" ref="N3:N7" si="0" xml:space="preserve"> 0.5*0.001</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O3" s="46" t="s">
+      <c r="O3" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P3" s="46" t="s">
+      <c r="P3" s="45" t="s">
         <v>198</v>
       </c>
-      <c r="Q3" s="46" t="s">
+      <c r="Q3" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="R3" s="46">
+      <c r="R3" s="45">
         <v>0</v>
       </c>
       <c r="T3">
@@ -4380,56 +4380,56 @@
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="46">
+      <c r="B4" s="45">
         <v>2</v>
       </c>
-      <c r="C4" s="46" t="s">
+      <c r="C4" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="46">
-        <v>0</v>
-      </c>
-      <c r="G4" s="46">
-        <v>0</v>
-      </c>
-      <c r="H4" s="46">
-        <v>0</v>
-      </c>
-      <c r="I4" s="46" t="s">
+      <c r="F4" s="45">
+        <v>0</v>
+      </c>
+      <c r="G4" s="45">
+        <v>0</v>
+      </c>
+      <c r="H4" s="45">
+        <v>0</v>
+      </c>
+      <c r="I4" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L4" s="46">
-        <v>0</v>
-      </c>
-      <c r="M4" s="46">
-        <v>0</v>
-      </c>
-      <c r="N4" s="46">
+      <c r="L4" s="45">
+        <v>0</v>
+      </c>
+      <c r="M4" s="45">
+        <v>0</v>
+      </c>
+      <c r="N4" s="45">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O4" s="46" t="s">
+      <c r="O4" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P4" s="46" t="s">
+      <c r="P4" s="45" t="s">
         <v>199</v>
       </c>
-      <c r="Q4" s="46" t="s">
+      <c r="Q4" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="R4" s="46">
+      <c r="R4" s="45">
         <v>0</v>
       </c>
       <c r="T4">
@@ -4443,56 +4443,56 @@
       <c r="A5" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="46">
+      <c r="B5" s="45">
         <v>2</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="46">
-        <v>0</v>
-      </c>
-      <c r="G5" s="46">
-        <v>0</v>
-      </c>
-      <c r="H5" s="46">
-        <v>0</v>
-      </c>
-      <c r="I5" s="46" t="s">
+      <c r="F5" s="45">
+        <v>0</v>
+      </c>
+      <c r="G5" s="45">
+        <v>0</v>
+      </c>
+      <c r="H5" s="45">
+        <v>0</v>
+      </c>
+      <c r="I5" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="K5" s="46" t="s">
+      <c r="K5" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L5" s="46">
-        <v>0</v>
-      </c>
-      <c r="M5" s="46">
-        <v>0</v>
-      </c>
-      <c r="N5" s="46">
+      <c r="L5" s="45">
+        <v>0</v>
+      </c>
+      <c r="M5" s="45">
+        <v>0</v>
+      </c>
+      <c r="N5" s="45">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O5" s="46" t="s">
+      <c r="O5" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P5" s="46" t="s">
+      <c r="P5" s="45" t="s">
         <v>200</v>
       </c>
-      <c r="Q5" s="46" t="s">
+      <c r="Q5" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="46">
+      <c r="R5" s="45">
         <v>0</v>
       </c>
       <c r="T5">
@@ -4506,56 +4506,56 @@
       <c r="A6" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="46">
+      <c r="B6" s="45">
         <v>2</v>
       </c>
-      <c r="C6" s="46" t="s">
+      <c r="C6" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E6" s="46" t="s">
+      <c r="E6" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="46">
-        <v>0</v>
-      </c>
-      <c r="G6" s="46">
-        <v>0</v>
-      </c>
-      <c r="H6" s="46">
-        <v>0</v>
-      </c>
-      <c r="I6" s="46" t="s">
+      <c r="F6" s="45">
+        <v>0</v>
+      </c>
+      <c r="G6" s="45">
+        <v>0</v>
+      </c>
+      <c r="H6" s="45">
+        <v>0</v>
+      </c>
+      <c r="I6" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="K6" s="46" t="s">
+      <c r="K6" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="46">
-        <v>0</v>
-      </c>
-      <c r="M6" s="46">
-        <v>0</v>
-      </c>
-      <c r="N6" s="46">
+      <c r="L6" s="45">
+        <v>0</v>
+      </c>
+      <c r="M6" s="45">
+        <v>0</v>
+      </c>
+      <c r="N6" s="45">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O6" s="46" t="s">
+      <c r="O6" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P6" s="46" t="s">
+      <c r="P6" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="Q6" s="46" t="s">
+      <c r="Q6" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="R6" s="46">
+      <c r="R6" s="45">
         <v>0</v>
       </c>
       <c r="T6">
@@ -4569,56 +4569,56 @@
       <c r="A7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="45">
         <v>2</v>
       </c>
-      <c r="C7" s="46" t="s">
+      <c r="C7" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="E7" s="46" t="s">
+      <c r="E7" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="48">
-        <v>0</v>
-      </c>
-      <c r="G7" s="46">
-        <v>0</v>
-      </c>
-      <c r="H7" s="46">
-        <v>0</v>
-      </c>
-      <c r="I7" s="46" t="s">
+      <c r="F7" s="47">
+        <v>0</v>
+      </c>
+      <c r="G7" s="45">
+        <v>0</v>
+      </c>
+      <c r="H7" s="45">
+        <v>0</v>
+      </c>
+      <c r="I7" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="46" t="s">
+      <c r="K7" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L7" s="48" t="s">
+      <c r="L7" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="48" t="s">
+      <c r="M7" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="N7" s="46">
+      <c r="N7" s="45">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O7" s="46" t="s">
+      <c r="O7" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P7" s="46" t="s">
+      <c r="P7" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="Q7" s="46" t="s">
+      <c r="Q7" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="R7" s="46">
+      <c r="R7" s="45">
         <v>0</v>
       </c>
       <c r="T7">
@@ -4632,55 +4632,55 @@
       <c r="A8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="45">
         <v>3</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="46" t="s">
+      <c r="E8" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="46">
-        <v>0</v>
-      </c>
-      <c r="G8" s="46" t="s">
+      <c r="F8" s="45">
+        <v>0</v>
+      </c>
+      <c r="G8" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>1</v>
       </c>
-      <c r="I8" s="46" t="s">
+      <c r="I8" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="J8" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="46" t="s">
+      <c r="K8" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L8" s="46">
-        <v>0</v>
-      </c>
-      <c r="M8" s="48">
-        <v>0</v>
-      </c>
-      <c r="N8" s="46">
-        <v>0.05</v>
-      </c>
-      <c r="O8" s="46" t="s">
+      <c r="L8" s="45">
+        <v>0</v>
+      </c>
+      <c r="M8" s="47">
+        <v>0</v>
+      </c>
+      <c r="N8" s="45">
+        <v>0</v>
+      </c>
+      <c r="O8" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P8" s="46">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="46" t="s">
+      <c r="P8" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="R8" s="46">
+      <c r="R8" s="45">
         <v>0</v>
       </c>
       <c r="T8">
@@ -4694,56 +4694,55 @@
       <c r="A9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="46">
+      <c r="B9" s="45">
         <v>3</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="46">
-        <v>0</v>
-      </c>
-      <c r="G9" s="46">
-        <v>0</v>
-      </c>
-      <c r="H9" s="46">
-        <v>0</v>
-      </c>
-      <c r="I9" s="46" t="s">
+      <c r="F9" s="45">
+        <v>0</v>
+      </c>
+      <c r="G9" s="45">
+        <v>0</v>
+      </c>
+      <c r="H9" s="45">
+        <v>0</v>
+      </c>
+      <c r="I9" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="J9" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="46" t="s">
+      <c r="K9" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="46">
-        <v>0</v>
-      </c>
-      <c r="M9" s="48">
-        <v>0</v>
-      </c>
-      <c r="N9" s="46">
-        <f>2.5*10^(-3)</f>
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="O9" s="46" t="s">
+      <c r="L9" s="45">
+        <v>0</v>
+      </c>
+      <c r="M9" s="47">
+        <v>0</v>
+      </c>
+      <c r="N9" s="45">
+        <v>0</v>
+      </c>
+      <c r="O9" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P9" s="46">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="46" t="s">
+      <c r="P9" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="R9" s="46">
+      <c r="R9" s="45">
         <v>0</v>
       </c>
       <c r="T9">
@@ -4757,55 +4756,55 @@
       <c r="A10" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="46">
+      <c r="B10" s="45">
         <v>4</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="46">
-        <v>0</v>
-      </c>
-      <c r="G10" s="46">
-        <v>0</v>
-      </c>
-      <c r="H10" s="50">
-        <v>0</v>
-      </c>
-      <c r="I10" s="46" t="s">
+      <c r="F10" s="45">
+        <v>0</v>
+      </c>
+      <c r="G10" s="45">
+        <v>0</v>
+      </c>
+      <c r="H10" s="49">
+        <v>0</v>
+      </c>
+      <c r="I10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="46" t="s">
+      <c r="J10" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="46" t="s">
+      <c r="K10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="46">
-        <v>0</v>
-      </c>
-      <c r="M10" s="48">
-        <v>0</v>
-      </c>
-      <c r="N10" s="48">
-        <v>0.08</v>
-      </c>
-      <c r="O10" s="46" t="s">
+      <c r="L10" s="45">
+        <v>0</v>
+      </c>
+      <c r="M10" s="47">
+        <v>0</v>
+      </c>
+      <c r="N10" s="47">
+        <v>1.2</v>
+      </c>
+      <c r="O10" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P10" s="46">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="46" t="s">
+      <c r="P10" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="R10" s="46">
+      <c r="R10" s="45">
         <v>0</v>
       </c>
       <c r="T10">
@@ -4819,55 +4818,55 @@
       <c r="A11" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="46">
+      <c r="B11" s="45">
         <v>5</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="46" t="s">
+      <c r="E11" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="46">
-        <v>0</v>
-      </c>
-      <c r="G11" s="46">
-        <v>0</v>
-      </c>
-      <c r="H11" s="46">
-        <v>0</v>
-      </c>
-      <c r="I11" s="46" t="s">
+      <c r="F11" s="45">
+        <v>0</v>
+      </c>
+      <c r="G11" s="45">
+        <v>0</v>
+      </c>
+      <c r="H11" s="45">
+        <v>0</v>
+      </c>
+      <c r="I11" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="46" t="s">
+      <c r="J11" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="46" t="s">
+      <c r="K11" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L11" s="46">
-        <v>0</v>
-      </c>
-      <c r="M11" s="48">
-        <v>0</v>
-      </c>
-      <c r="N11" s="46">
-        <v>0.08</v>
-      </c>
-      <c r="O11" s="46" t="s">
+      <c r="L11" s="45">
+        <v>0</v>
+      </c>
+      <c r="M11" s="47">
+        <v>0</v>
+      </c>
+      <c r="N11" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="O11" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P11" s="46">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="46" t="s">
+      <c r="P11" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="R11" s="46">
+      <c r="R11" s="45">
         <v>0</v>
       </c>
       <c r="T11" t="s">
@@ -4881,55 +4880,55 @@
       <c r="A12" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="46">
+      <c r="B12" s="45">
         <v>6</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="46" t="s">
+      <c r="E12" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="46">
-        <v>0</v>
-      </c>
-      <c r="G12" s="46">
-        <v>0</v>
-      </c>
-      <c r="H12" s="46">
-        <v>0</v>
-      </c>
-      <c r="I12" s="46" t="s">
+      <c r="F12" s="45">
+        <v>0</v>
+      </c>
+      <c r="G12" s="45">
+        <v>0</v>
+      </c>
+      <c r="H12" s="45">
+        <v>0</v>
+      </c>
+      <c r="I12" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="46" t="s">
+      <c r="J12" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="46" t="s">
+      <c r="K12" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="L12" s="46">
-        <v>0</v>
-      </c>
-      <c r="M12" s="48">
-        <v>0</v>
-      </c>
-      <c r="N12" s="46">
-        <v>0.08</v>
-      </c>
-      <c r="O12" s="46" t="s">
+      <c r="L12" s="45">
+        <v>0</v>
+      </c>
+      <c r="M12" s="47">
+        <v>0</v>
+      </c>
+      <c r="N12" s="45">
+        <v>0</v>
+      </c>
+      <c r="O12" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="P12" s="46">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="46" t="s">
+      <c r="P12" s="45">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="R12" s="46">
+      <c r="R12" s="45">
         <v>0</v>
       </c>
       <c r="T12">
@@ -5436,7 +5435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BC952C-F64C-4F30-9DDA-924F82AF01AE}">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="S22" sqref="S22"/>
     </sheetView>
@@ -6285,7 +6284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8D8FB7-0FD2-42C3-9D82-0A6D9AE32488}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A2" sqref="A2:A6"/>
     </sheetView>
@@ -6484,38 +6483,38 @@
       <c r="B7" s="34">
         <v>0</v>
       </c>
-      <c r="C7" s="41">
-        <v>0</v>
-      </c>
-      <c r="D7" s="41" t="s">
+      <c r="C7" s="40">
+        <v>0</v>
+      </c>
+      <c r="D7" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="F7" s="41" t="s">
+      <c r="F7" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="G7" s="42">
+      <c r="G7" s="41">
         <v>0</v>
       </c>
       <c r="H7" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="41" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="25"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
     </row>
     <row r="9" spans="1:9">
       <c r="H9" s="30"/>

</xml_diff>

<commit_message>
add distilation_3 model DOne
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v2.xlsx
+++ b/excel files/propionate_case_study_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF62FEC5-EF7B-4EEF-A34D-2E56D66846FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6B891E-EF7E-40EC-8997-BB040ADF59FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="249">
   <si>
     <t>components</t>
   </si>
@@ -823,12 +823,15 @@
   <si>
     <t>Distillation_2.json</t>
   </si>
+  <si>
+    <t>Distillation_3.json</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -876,13 +879,6 @@
       <color rgb="FF008000"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1006,7 +1002,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -1074,21 +1070,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1113,9 +1094,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1181,13 +1162,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1202,21 +1180,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1225,10 +1203,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2431,16 +2409,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>622618</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>129008</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>773430</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9946</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>195686</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>424</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>92499</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>63924</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2455,8 +2433,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9687243" y="3248446"/>
-          <a:ext cx="3557693" cy="3705228"/>
+          <a:off x="10639743" y="2930946"/>
+          <a:ext cx="3835506" cy="3705228"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2573,13 +2551,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>160654</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>46036</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>936625</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>7937</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2656,15 +2634,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>200872</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>139594</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>76202</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2802,22 +2780,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>119062</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>45708</xdr:rowOff>
+      <xdr:colOff>105901</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>150811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>611188</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>21748</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>56740</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>81076</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="58" name="Picture 57">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD857D0A-2125-75AD-2D4B-0F87877E81A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBF62936-21DA-FE1A-A014-6C9C17368E44}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2833,8 +2811,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3159125" y="3165146"/>
-          <a:ext cx="6516688" cy="3079602"/>
+          <a:off x="3145964" y="3270249"/>
+          <a:ext cx="7578776" cy="3581515"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3705,7 +3683,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3762,13 +3740,13 @@
       <c r="D2" s="4">
         <v>1000</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>214</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="38" t="s">
         <v>214</v>
       </c>
       <c r="H2" s="4">
@@ -4008,10 +3986,10 @@
       <c r="C11" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="42" t="s">
         <v>217</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="43"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="30" t="s">
@@ -4026,10 +4004,10 @@
       <c r="D12" t="s">
         <v>218</v>
       </c>
-      <c r="E12" s="44"/>
+      <c r="E12" s="43"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="44"/>
+      <c r="A14" s="43"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4083,10 +4061,10 @@
       <c r="C2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="43" t="s">
+      <c r="D2" s="42" t="s">
         <v>237</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>238</v>
       </c>
       <c r="F2" t="s">
@@ -4157,9 +4135,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N12" sqref="N12"/>
+      <selection pane="topRight" activeCell="N9" sqref="N9:N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4192,55 +4170,55 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="47" t="s">
         <v>122</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="47" t="s">
         <v>73</v>
       </c>
       <c r="T1" s="18" t="s">
@@ -4254,56 +4232,56 @@
       <c r="A2" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="45">
+      <c r="B2" s="44">
         <v>2</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="45">
-        <v>0</v>
-      </c>
-      <c r="G2" s="45">
-        <v>0</v>
-      </c>
-      <c r="H2" s="45">
-        <v>0</v>
-      </c>
-      <c r="I2" s="45" t="s">
+      <c r="F2" s="44">
+        <v>0</v>
+      </c>
+      <c r="G2" s="44">
+        <v>0</v>
+      </c>
+      <c r="H2" s="44">
+        <v>0</v>
+      </c>
+      <c r="I2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="K2" s="45" t="s">
+      <c r="K2" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="47">
-        <v>0</v>
-      </c>
-      <c r="M2" s="45">
-        <v>0</v>
-      </c>
-      <c r="N2" s="45">
+      <c r="L2" s="46">
+        <v>0</v>
+      </c>
+      <c r="M2" s="44">
+        <v>0</v>
+      </c>
+      <c r="N2" s="44">
         <f xml:space="preserve"> 0.5*0.001</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O2" s="45" t="s">
+      <c r="O2" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="44" t="s">
         <v>197</v>
       </c>
-      <c r="Q2" s="45" t="s">
+      <c r="Q2" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="R2" s="45">
+      <c r="R2" s="44">
         <v>0</v>
       </c>
       <c r="T2">
@@ -4317,56 +4295,56 @@
       <c r="A3" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="44">
         <v>2</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="45">
-        <v>0</v>
-      </c>
-      <c r="G3" s="45">
-        <v>0</v>
-      </c>
-      <c r="H3" s="45">
-        <v>0</v>
-      </c>
-      <c r="I3" s="45" t="s">
+      <c r="F3" s="44">
+        <v>0</v>
+      </c>
+      <c r="G3" s="44">
+        <v>0</v>
+      </c>
+      <c r="H3" s="44">
+        <v>0</v>
+      </c>
+      <c r="I3" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J3" s="45" t="s">
+      <c r="J3" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="K3" s="45" t="s">
+      <c r="K3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L3" s="45">
-        <v>0</v>
-      </c>
-      <c r="M3" s="45">
-        <v>0</v>
-      </c>
-      <c r="N3" s="45">
+      <c r="L3" s="44">
+        <v>0</v>
+      </c>
+      <c r="M3" s="44">
+        <v>0</v>
+      </c>
+      <c r="N3" s="44">
         <f t="shared" ref="N3:N7" si="0" xml:space="preserve"> 0.5*0.001</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O3" s="45" t="s">
+      <c r="O3" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P3" s="45" t="s">
+      <c r="P3" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="Q3" s="45" t="s">
+      <c r="Q3" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="R3" s="45">
+      <c r="R3" s="44">
         <v>0</v>
       </c>
       <c r="T3">
@@ -4380,56 +4358,56 @@
       <c r="A4" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="45">
+      <c r="B4" s="44">
         <v>2</v>
       </c>
-      <c r="C4" s="45" t="s">
+      <c r="C4" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="45">
-        <v>0</v>
-      </c>
-      <c r="G4" s="45">
-        <v>0</v>
-      </c>
-      <c r="H4" s="45">
-        <v>0</v>
-      </c>
-      <c r="I4" s="45" t="s">
+      <c r="F4" s="44">
+        <v>0</v>
+      </c>
+      <c r="G4" s="44">
+        <v>0</v>
+      </c>
+      <c r="H4" s="44">
+        <v>0</v>
+      </c>
+      <c r="I4" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="45" t="s">
+      <c r="J4" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="K4" s="45" t="s">
+      <c r="K4" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L4" s="45">
-        <v>0</v>
-      </c>
-      <c r="M4" s="45">
-        <v>0</v>
-      </c>
-      <c r="N4" s="45">
+      <c r="L4" s="44">
+        <v>0</v>
+      </c>
+      <c r="M4" s="44">
+        <v>0</v>
+      </c>
+      <c r="N4" s="44">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O4" s="45" t="s">
+      <c r="O4" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P4" s="45" t="s">
+      <c r="P4" s="44" t="s">
         <v>199</v>
       </c>
-      <c r="Q4" s="45" t="s">
+      <c r="Q4" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="R4" s="45">
+      <c r="R4" s="44">
         <v>0</v>
       </c>
       <c r="T4">
@@ -4443,56 +4421,56 @@
       <c r="A5" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="44">
         <v>2</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="45">
-        <v>0</v>
-      </c>
-      <c r="G5" s="45">
-        <v>0</v>
-      </c>
-      <c r="H5" s="45">
-        <v>0</v>
-      </c>
-      <c r="I5" s="45" t="s">
+      <c r="F5" s="44">
+        <v>0</v>
+      </c>
+      <c r="G5" s="44">
+        <v>0</v>
+      </c>
+      <c r="H5" s="44">
+        <v>0</v>
+      </c>
+      <c r="I5" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J5" s="45" t="s">
+      <c r="J5" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="K5" s="45" t="s">
+      <c r="K5" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L5" s="45">
-        <v>0</v>
-      </c>
-      <c r="M5" s="45">
-        <v>0</v>
-      </c>
-      <c r="N5" s="45">
+      <c r="L5" s="44">
+        <v>0</v>
+      </c>
+      <c r="M5" s="44">
+        <v>0</v>
+      </c>
+      <c r="N5" s="44">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O5" s="45" t="s">
+      <c r="O5" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P5" s="45" t="s">
+      <c r="P5" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="Q5" s="45" t="s">
+      <c r="Q5" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="R5" s="45">
+      <c r="R5" s="44">
         <v>0</v>
       </c>
       <c r="T5">
@@ -4506,56 +4484,56 @@
       <c r="A6" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="44">
         <v>2</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="45">
-        <v>0</v>
-      </c>
-      <c r="G6" s="45">
-        <v>0</v>
-      </c>
-      <c r="H6" s="45">
-        <v>0</v>
-      </c>
-      <c r="I6" s="45" t="s">
+      <c r="F6" s="44">
+        <v>0</v>
+      </c>
+      <c r="G6" s="44">
+        <v>0</v>
+      </c>
+      <c r="H6" s="44">
+        <v>0</v>
+      </c>
+      <c r="I6" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="45" t="s">
+      <c r="J6" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="K6" s="45" t="s">
+      <c r="K6" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L6" s="45">
-        <v>0</v>
-      </c>
-      <c r="M6" s="45">
-        <v>0</v>
-      </c>
-      <c r="N6" s="45">
+      <c r="L6" s="44">
+        <v>0</v>
+      </c>
+      <c r="M6" s="44">
+        <v>0</v>
+      </c>
+      <c r="N6" s="44">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O6" s="45" t="s">
+      <c r="O6" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P6" s="45" t="s">
+      <c r="P6" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="Q6" s="45" t="s">
+      <c r="Q6" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="R6" s="45">
+      <c r="R6" s="44">
         <v>0</v>
       </c>
       <c r="T6">
@@ -4569,56 +4547,56 @@
       <c r="A7" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="45">
+      <c r="B7" s="44">
         <v>2</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="47">
-        <v>0</v>
-      </c>
-      <c r="G7" s="45">
-        <v>0</v>
-      </c>
-      <c r="H7" s="45">
-        <v>0</v>
-      </c>
-      <c r="I7" s="45" t="s">
+      <c r="F7" s="46">
+        <v>0</v>
+      </c>
+      <c r="G7" s="44">
+        <v>0</v>
+      </c>
+      <c r="H7" s="44">
+        <v>0</v>
+      </c>
+      <c r="I7" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="K7" s="45" t="s">
+      <c r="K7" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L7" s="47" t="s">
+      <c r="L7" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="M7" s="47" t="s">
+      <c r="M7" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="N7" s="45">
+      <c r="N7" s="44">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="O7" s="45" t="s">
+      <c r="O7" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P7" s="45" t="s">
+      <c r="P7" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="Q7" s="45" t="s">
+      <c r="Q7" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="R7" s="45">
+      <c r="R7" s="44">
         <v>0</v>
       </c>
       <c r="T7">
@@ -4632,55 +4610,55 @@
       <c r="A8" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="45">
+      <c r="B8" s="44">
         <v>3</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D8" s="45" t="s">
+      <c r="D8" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="45" t="s">
+      <c r="E8" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="45">
-        <v>0</v>
-      </c>
-      <c r="G8" s="45" t="s">
+      <c r="F8" s="44">
+        <v>0</v>
+      </c>
+      <c r="G8" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="45">
+      <c r="H8" s="44">
         <v>1</v>
       </c>
-      <c r="I8" s="45" t="s">
+      <c r="I8" s="44" t="s">
         <v>91</v>
       </c>
-      <c r="J8" s="45" t="s">
+      <c r="J8" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="45" t="s">
+      <c r="K8" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L8" s="45">
-        <v>0</v>
-      </c>
-      <c r="M8" s="47">
-        <v>0</v>
-      </c>
-      <c r="N8" s="45">
-        <v>0</v>
-      </c>
-      <c r="O8" s="45" t="s">
+      <c r="L8" s="44">
+        <v>0</v>
+      </c>
+      <c r="M8" s="46">
+        <v>0</v>
+      </c>
+      <c r="N8" s="44">
+        <v>0</v>
+      </c>
+      <c r="O8" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P8" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="45" t="s">
+      <c r="P8" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="44" t="s">
         <v>109</v>
       </c>
-      <c r="R8" s="45">
+      <c r="R8" s="44">
         <v>0</v>
       </c>
       <c r="T8">
@@ -4694,55 +4672,55 @@
       <c r="A9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="44">
         <v>3</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="45">
-        <v>0</v>
-      </c>
-      <c r="G9" s="45">
-        <v>0</v>
-      </c>
-      <c r="H9" s="45">
-        <v>0</v>
-      </c>
-      <c r="I9" s="45" t="s">
+      <c r="F9" s="44">
+        <v>0</v>
+      </c>
+      <c r="G9" s="44">
+        <v>0</v>
+      </c>
+      <c r="H9" s="44">
+        <v>0</v>
+      </c>
+      <c r="I9" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J9" s="45" t="s">
+      <c r="J9" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="K9" s="45" t="s">
+      <c r="K9" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L9" s="45">
-        <v>0</v>
-      </c>
-      <c r="M9" s="47">
-        <v>0</v>
-      </c>
-      <c r="N9" s="45">
-        <v>0</v>
-      </c>
-      <c r="O9" s="45" t="s">
+      <c r="L9" s="44">
+        <v>0</v>
+      </c>
+      <c r="M9" s="46">
+        <v>0</v>
+      </c>
+      <c r="N9" s="44">
+        <v>0</v>
+      </c>
+      <c r="O9" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P9" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="45" t="s">
+      <c r="P9" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="R9" s="45">
+      <c r="R9" s="44">
         <v>0</v>
       </c>
       <c r="T9">
@@ -4756,55 +4734,55 @@
       <c r="A10" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="45">
+      <c r="B10" s="44">
         <v>4</v>
       </c>
-      <c r="C10" s="45" t="s">
+      <c r="C10" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="45" t="s">
+      <c r="E10" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F10" s="45">
-        <v>0</v>
-      </c>
-      <c r="G10" s="45">
-        <v>0</v>
-      </c>
-      <c r="H10" s="49">
-        <v>0</v>
-      </c>
-      <c r="I10" s="45" t="s">
+      <c r="F10" s="44">
+        <v>0</v>
+      </c>
+      <c r="G10" s="44">
+        <v>0</v>
+      </c>
+      <c r="H10" s="48">
+        <v>0</v>
+      </c>
+      <c r="I10" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="J10" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="K10" s="45" t="s">
+      <c r="K10" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L10" s="45">
-        <v>0</v>
-      </c>
-      <c r="M10" s="47">
-        <v>0</v>
-      </c>
-      <c r="N10" s="47">
+      <c r="L10" s="44">
+        <v>0</v>
+      </c>
+      <c r="M10" s="46">
+        <v>0</v>
+      </c>
+      <c r="N10" s="46">
         <v>1.2</v>
       </c>
-      <c r="O10" s="45" t="s">
+      <c r="O10" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P10" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="45" t="s">
+      <c r="P10" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="R10" s="45">
+      <c r="R10" s="44">
         <v>0</v>
       </c>
       <c r="T10">
@@ -4818,55 +4796,55 @@
       <c r="A11" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="45">
+      <c r="B11" s="44">
         <v>5</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="E11" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="45">
-        <v>0</v>
-      </c>
-      <c r="G11" s="45">
-        <v>0</v>
-      </c>
-      <c r="H11" s="45">
-        <v>0</v>
-      </c>
-      <c r="I11" s="45" t="s">
+      <c r="F11" s="44">
+        <v>0</v>
+      </c>
+      <c r="G11" s="44">
+        <v>0</v>
+      </c>
+      <c r="H11" s="44">
+        <v>0</v>
+      </c>
+      <c r="I11" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="J11" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="K11" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L11" s="45">
-        <v>0</v>
-      </c>
-      <c r="M11" s="47">
-        <v>0</v>
-      </c>
-      <c r="N11" s="45" t="s">
+      <c r="L11" s="44">
+        <v>0</v>
+      </c>
+      <c r="M11" s="46">
+        <v>0</v>
+      </c>
+      <c r="N11" s="44" t="s">
         <v>247</v>
       </c>
-      <c r="O11" s="45" t="s">
+      <c r="O11" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P11" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="45" t="s">
+      <c r="P11" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="R11" s="45">
+      <c r="R11" s="44">
         <v>0</v>
       </c>
       <c r="T11" t="s">
@@ -4880,55 +4858,55 @@
       <c r="A12" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="45">
+      <c r="B12" s="44">
         <v>6</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F12" s="45">
-        <v>0</v>
-      </c>
-      <c r="G12" s="45">
-        <v>0</v>
-      </c>
-      <c r="H12" s="45">
-        <v>0</v>
-      </c>
-      <c r="I12" s="45" t="s">
+      <c r="F12" s="44">
+        <v>0</v>
+      </c>
+      <c r="G12" s="44">
+        <v>0</v>
+      </c>
+      <c r="H12" s="44">
+        <v>0</v>
+      </c>
+      <c r="I12" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="J12" s="45" t="s">
+      <c r="J12" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="45" t="s">
+      <c r="K12" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="L12" s="45">
-        <v>0</v>
-      </c>
-      <c r="M12" s="47">
-        <v>0</v>
-      </c>
-      <c r="N12" s="45">
-        <v>0</v>
-      </c>
-      <c r="O12" s="45" t="s">
+      <c r="L12" s="44">
+        <v>0</v>
+      </c>
+      <c r="M12" s="46">
+        <v>0</v>
+      </c>
+      <c r="N12" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="O12" s="44" t="s">
         <v>176</v>
       </c>
-      <c r="P12" s="45">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="45" t="s">
+      <c r="P12" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="R12" s="45">
+      <c r="R12" s="44">
         <v>0</v>
       </c>
       <c r="T12">
@@ -5433,11 +5411,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BC952C-F64C-4F30-9DDA-924F82AF01AE}">
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="S22" sqref="S22"/>
+      <selection pane="topRight" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -5450,32 +5428,32 @@
     <col min="7" max="7" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="34" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="34" t="s">
         <v>45</v>
       </c>
       <c r="I1" s="20" t="s">
@@ -5485,26 +5463,23 @@
         <v>54</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="M1" s="20" t="s">
         <v>116</v>
       </c>
+      <c r="M1" s="23" t="s">
+        <v>19</v>
+      </c>
       <c r="N1" s="23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:15">
+      <c r="A2" s="35" t="s">
         <v>213</v>
       </c>
       <c r="B2" s="14">
@@ -5549,12 +5524,9 @@
       <c r="O2" s="9">
         <v>0</v>
       </c>
-      <c r="P2" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="35" t="s">
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" s="34" t="s">
         <v>117</v>
       </c>
       <c r="B3" s="9">
@@ -5596,15 +5568,12 @@
       <c r="N3" s="9">
         <v>0</v>
       </c>
-      <c r="O3" s="9">
-        <v>0</v>
-      </c>
-      <c r="P3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:15">
+      <c r="A4" s="34" t="s">
         <v>118</v>
       </c>
       <c r="B4" s="9">
@@ -5646,15 +5615,12 @@
       <c r="N4" s="9">
         <v>0</v>
       </c>
-      <c r="O4" s="9">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:15">
+      <c r="A5" s="34" t="s">
         <v>119</v>
       </c>
       <c r="B5" s="9">
@@ -5684,27 +5650,24 @@
       <c r="J5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="37">
-        <v>0</v>
-      </c>
-      <c r="L5" s="37">
-        <v>0</v>
-      </c>
-      <c r="M5" s="37">
+      <c r="K5" s="36">
+        <v>0</v>
+      </c>
+      <c r="L5" s="36">
+        <v>0</v>
+      </c>
+      <c r="M5" s="9">
         <v>0</v>
       </c>
       <c r="N5" s="9">
         <v>0</v>
       </c>
-      <c r="O5" s="9">
-        <v>0</v>
-      </c>
-      <c r="P5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:15">
+      <c r="A6" s="34" t="s">
         <v>120</v>
       </c>
       <c r="B6" s="9">
@@ -5746,15 +5709,12 @@
       <c r="N6" s="9">
         <v>0</v>
       </c>
-      <c r="O6" s="9">
-        <v>0</v>
-      </c>
-      <c r="P6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:15">
+      <c r="A7" s="34" t="s">
         <v>121</v>
       </c>
       <c r="B7" s="9">
@@ -5796,15 +5756,12 @@
       <c r="N7" s="9">
         <v>0</v>
       </c>
-      <c r="O7" s="9">
-        <v>0</v>
-      </c>
-      <c r="P7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:15">
+      <c r="A8" s="34" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="9">
@@ -5846,14 +5803,11 @@
       <c r="N8" s="9">
         <v>0</v>
       </c>
-      <c r="O8" s="9">
-        <v>0</v>
-      </c>
-      <c r="P8" s="6" t="s">
+      <c r="O8" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:15">
       <c r="A9" s="22" t="s">
         <v>53</v>
       </c>
@@ -5884,8 +5838,8 @@
       <c r="J9" s="9">
         <v>0</v>
       </c>
-      <c r="K9" s="6" t="s">
-        <v>23</v>
+      <c r="K9" s="9">
+        <v>0</v>
       </c>
       <c r="L9" s="9">
         <v>0</v>
@@ -5896,14 +5850,11 @@
       <c r="N9" s="9">
         <v>0</v>
       </c>
-      <c r="O9" s="9">
-        <v>0</v>
-      </c>
-      <c r="P9" s="6" t="s">
+      <c r="O9" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1">
+    <row r="10" spans="1:15">
       <c r="A10" s="22" t="s">
         <v>54</v>
       </c>
@@ -5928,34 +5879,31 @@
       <c r="H10" s="9">
         <v>0</v>
       </c>
-      <c r="I10" s="38">
+      <c r="I10" s="37">
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="K10" s="9">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6" t="s">
+      <c r="K10" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
       <c r="M10" s="9">
         <v>0</v>
       </c>
       <c r="N10" s="9">
         <v>0</v>
       </c>
-      <c r="O10" s="9">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6" t="s">
+      <c r="O10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" thickBot="1">
+    <row r="11" spans="1:15">
       <c r="A11" s="22" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -5975,37 +5923,34 @@
       <c r="G11" s="9">
         <v>0</v>
       </c>
-      <c r="H11" s="16">
-        <v>0</v>
-      </c>
-      <c r="I11" s="16">
-        <v>0</v>
-      </c>
-      <c r="J11" s="16">
+      <c r="H11" s="9">
+        <v>0</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9">
         <v>0</v>
       </c>
       <c r="K11" s="9">
         <v>0</v>
       </c>
-      <c r="L11" s="9">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6" t="s">
+      <c r="L11" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="M11" s="9">
+        <v>0</v>
+      </c>
       <c r="N11" s="9">
         <v>0</v>
       </c>
-      <c r="O11" s="9">
-        <v>0</v>
-      </c>
-      <c r="P11" s="32" t="s">
+      <c r="O11" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:15">
       <c r="A12" s="22" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B12" s="9">
         <v>0</v>
@@ -6043,19 +5988,16 @@
       <c r="M12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="9">
-        <v>0</v>
+      <c r="N12" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="O12" s="9">
         <v>0</v>
       </c>
-      <c r="P12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="22" t="s">
-        <v>116</v>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="23" t="s">
+        <v>19</v>
       </c>
       <c r="B13" s="9">
         <v>0</v>
@@ -6093,19 +6035,16 @@
       <c r="M13" s="9">
         <v>0</v>
       </c>
-      <c r="N13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="N13" s="9">
+        <v>0</v>
+      </c>
+      <c r="O13" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" s="9">
         <v>0</v>
@@ -6149,13 +6088,10 @@
       <c r="O14" s="9">
         <v>0</v>
       </c>
-      <c r="P14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="23" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
@@ -6199,63 +6135,10 @@
       <c r="O15" s="9">
         <v>0</v>
       </c>
-      <c r="P15" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="5">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9">
-        <v>0</v>
-      </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="9">
-        <v>0</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0</v>
-      </c>
-      <c r="K16" s="9">
-        <v>0</v>
-      </c>
-      <c r="L16" s="9">
-        <v>0</v>
-      </c>
-      <c r="M16" s="9">
-        <v>0</v>
-      </c>
-      <c r="N16" s="9">
-        <v>0</v>
-      </c>
-      <c r="O16" s="9">
-        <v>0</v>
-      </c>
-      <c r="P16" s="9">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B3:B8 B9:P16 C4:C7 C8:G8 C2:P2 D5:D7 D3:H3 E4 E6:E7 F4:F5 F7 G4:G6 H4:H7 I3:P8">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C3 D4 E5 F6 G7 H8">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6264,8 +6147,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3 D4 E5 F6 G7 H8">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="B3:B8 B9:O15 C4:C7 C8:G8 C2:O2 D5:D7 D3:H3 E4 E6:E7 F4:F5 F7 G4:G6 H4:H7 I3:O8">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -6335,19 +6218,19 @@
       <c r="A2" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="34">
-        <v>0</v>
-      </c>
-      <c r="D2" s="34">
-        <v>0</v>
-      </c>
-      <c r="E2" s="34">
-        <v>0</v>
-      </c>
-      <c r="F2" s="34">
+      <c r="C2" s="33">
+        <v>0</v>
+      </c>
+      <c r="D2" s="33">
+        <v>0</v>
+      </c>
+      <c r="E2" s="33">
+        <v>0</v>
+      </c>
+      <c r="F2" s="33">
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
@@ -6364,19 +6247,19 @@
       <c r="A3" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C3" s="34">
-        <v>0</v>
-      </c>
-      <c r="D3" s="34">
-        <v>0</v>
-      </c>
-      <c r="E3" s="34">
-        <v>0</v>
-      </c>
-      <c r="F3" s="34">
+      <c r="C3" s="33">
+        <v>0</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0</v>
+      </c>
+      <c r="F3" s="33">
         <v>0</v>
       </c>
       <c r="G3" s="13" t="s">
@@ -6393,19 +6276,19 @@
       <c r="A4" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="34">
-        <v>0</v>
-      </c>
-      <c r="D4" s="34">
-        <v>0</v>
-      </c>
-      <c r="E4" s="34">
-        <v>0</v>
-      </c>
-      <c r="F4" s="34">
+      <c r="C4" s="33">
+        <v>0</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0</v>
+      </c>
+      <c r="F4" s="33">
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
@@ -6422,19 +6305,19 @@
       <c r="A5" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="34">
-        <v>0</v>
-      </c>
-      <c r="D5" s="34">
-        <v>0</v>
-      </c>
-      <c r="E5" s="34">
-        <v>0</v>
-      </c>
-      <c r="F5" s="34">
+      <c r="C5" s="33">
+        <v>0</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="33">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33">
         <v>0</v>
       </c>
       <c r="G5" s="13" t="s">
@@ -6451,19 +6334,19 @@
       <c r="A6" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="34">
-        <v>0</v>
-      </c>
-      <c r="D6" s="34">
-        <v>0</v>
-      </c>
-      <c r="E6" s="34">
-        <v>0</v>
-      </c>
-      <c r="F6" s="34">
+      <c r="C6" s="33">
+        <v>0</v>
+      </c>
+      <c r="D6" s="33">
+        <v>0</v>
+      </c>
+      <c r="E6" s="33">
+        <v>0</v>
+      </c>
+      <c r="F6" s="33">
         <v>0</v>
       </c>
       <c r="G6" s="13" t="s">
@@ -6480,41 +6363,41 @@
       <c r="A7" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B7" s="34">
-        <v>0</v>
-      </c>
-      <c r="C7" s="40">
-        <v>0</v>
-      </c>
-      <c r="D7" s="40" t="s">
+      <c r="B7" s="33">
+        <v>0</v>
+      </c>
+      <c r="C7" s="39">
+        <v>0</v>
+      </c>
+      <c r="D7" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="39" t="s">
         <v>210</v>
       </c>
-      <c r="G7" s="41">
+      <c r="G7" s="40">
         <v>0</v>
       </c>
       <c r="H7" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="I7" s="41" t="s">
+      <c r="I7" s="40" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="25"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:9">
       <c r="H9" s="30"/>
@@ -7341,7 +7224,7 @@
       <c r="A13" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="32" t="s">
         <v>194</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -7370,7 +7253,7 @@
       <c r="A14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="33" t="s">
+      <c r="B14" s="32" t="s">
         <v>194</v>
       </c>
       <c r="C14" s="4" t="s">

</xml_diff>

<commit_message>
fix bug distillation units
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v2.xlsx
+++ b/excel files/propionate_case_study_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6B891E-EF7E-40EC-8997-BB040ADF59FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04EBE40-6266-43E0-8291-651E512C1588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="244">
   <si>
     <t>components</t>
   </si>
@@ -286,18 +286,12 @@
     <t>[0.01,  0.01, 0.98]</t>
   </si>
   <si>
-    <t>[0.01,  0.01, 0.01, 0.98]</t>
-  </si>
-  <si>
     <t>[0,  0]</t>
   </si>
   <si>
     <t>stream_reuse</t>
   </si>
   <si>
-    <t>ace,prop, Hoc, water</t>
-  </si>
-  <si>
     <t>{'Hoc' : 'liq_liq_ext' }</t>
   </si>
   <si>
@@ -331,9 +325,6 @@
     <t>{'pH':[5,8.5]}</t>
   </si>
   <si>
-    <t>Hoc, ace, prop, water</t>
-  </si>
-  <si>
     <t>ace, prop, water</t>
   </si>
   <si>
@@ -377,9 +368,6 @@
   </si>
   <si>
     <t>[0.95, 0.95, 0.05] ; [0.05, 0.05, 0.95]</t>
-  </si>
-  <si>
-    <t>[0.95, 0.95, 0.95, 0.05]; [0.05, 0.05, 0.05, 0.95]</t>
   </si>
   <si>
     <r>
@@ -399,9 +387,6 @@
   </si>
   <si>
     <t>[0.95, 0.05]; [0.05, 0.95]</t>
-  </si>
-  <si>
-    <t>Distilation_1</t>
   </si>
   <si>
     <t>Distilation_2</t>
@@ -1096,7 +1081,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1207,6 +1192,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1623,7 +1611,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>1172210</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2540</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1693,13 +1681,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>100330</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1780,7 +1768,7 @@
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>1231900</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1866,13 +1854,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>73660</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1111250</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>109220</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1941,13 +1929,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2042,13 +2030,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>240030</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>173990</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1277620</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>138430</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2112,13 +2100,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2203,14 +2191,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>93980</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1212850</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2225,8 +2213,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12463780" y="2622550"/>
-          <a:ext cx="1118870" cy="1066800"/>
+          <a:off x="12463780" y="2438400"/>
+          <a:ext cx="1334770" cy="1778000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2270,6 +2258,40 @@
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
             <a:t>eg: testDistilation.json</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Distillation_2.json</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Distillation_3.json</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB"/>
+            <a:t> </a:t>
+          </a:r>
           <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -2285,13 +2307,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>441961</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>53953</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>106680</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>25410</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2329,13 +2351,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>43180</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>99060</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1494790</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3683,7 +3705,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3732,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C2" s="4">
         <v>500</v>
@@ -3741,13 +3763,13 @@
         <v>1000</v>
       </c>
       <c r="E2" s="38" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F2" s="4">
         <v>0</v>
       </c>
       <c r="G2" s="38" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -3838,10 +3860,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -3852,7 +3874,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="30" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B2">
         <v>222</v>
@@ -3861,12 +3883,12 @@
         <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="30" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B3">
         <v>85.8</v>
@@ -3875,12 +3897,12 @@
         <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="30" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B4">
         <v>64.3</v>
@@ -3889,12 +3911,12 @@
         <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="30" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B5">
         <v>74.8</v>
@@ -3903,12 +3925,12 @@
         <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="30" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B6">
         <v>61.1</v>
@@ -3917,12 +3939,12 @@
         <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="30" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B7">
         <v>381</v>
@@ -3931,12 +3953,12 @@
         <v>61</v>
       </c>
       <c r="D7" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="30" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B8">
         <v>53.6</v>
@@ -3945,12 +3967,12 @@
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="30" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B9">
         <v>53.3</v>
@@ -3959,12 +3981,12 @@
         <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="30" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B10">
         <v>52.3</v>
@@ -3973,12 +3995,12 @@
         <v>61</v>
       </c>
       <c r="D10" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="30" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B11">
         <v>78.5</v>
@@ -3987,13 +4009,13 @@
         <v>61</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E11" s="43"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="30" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B12">
         <v>50.5</v>
@@ -4002,7 +4024,7 @@
         <v>61</v>
       </c>
       <c r="D12" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E12" s="43"/>
     </row>
@@ -4020,7 +4042,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4033,27 +4055,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" t="s">
         <v>239</v>
-      </c>
-      <c r="F1" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B2" s="4">
         <v>37</v>
@@ -4062,21 +4084,21 @@
         <v>70</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="E2" s="49" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="F2" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="C3" t="s">
         <v>70</v>
@@ -4084,31 +4106,31 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="B7" s="4">
         <v>71</v>
@@ -4117,10 +4139,10 @@
         <v>70</v>
       </c>
       <c r="D7" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="F7" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4133,11 +4155,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F85D0432-6958-423D-87F2-E8A979C87816}">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N9" sqref="N9:N10"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4171,19 +4193,19 @@
         <v>6</v>
       </c>
       <c r="B1" s="47" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C1" s="47" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D1" s="47" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E1" s="47" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F1" s="47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G1" s="47" t="s">
         <v>68</v>
@@ -4198,16 +4220,16 @@
         <v>15</v>
       </c>
       <c r="K1" s="47" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="M1" s="47" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="N1" s="47" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="O1" s="47" t="s">
         <v>60</v>
@@ -4222,7 +4244,7 @@
         <v>73</v>
       </c>
       <c r="T1" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>78</v>
@@ -4230,16 +4252,16 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="44">
         <v>2</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D2" s="45" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E2" s="44" t="s">
         <v>75</v>
@@ -4257,7 +4279,7 @@
         <v>72</v>
       </c>
       <c r="J2" s="44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K2" s="44" t="s">
         <v>75</v>
@@ -4273,13 +4295,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="O2" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P2" s="44" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="Q2" s="44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R2" s="44">
         <v>0</v>
@@ -4288,21 +4310,21 @@
         <v>0</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B3" s="44">
         <v>2</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D3" s="45" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E3" s="44" t="s">
         <v>75</v>
@@ -4320,7 +4342,7 @@
         <v>72</v>
       </c>
       <c r="J3" s="44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K3" s="44" t="s">
         <v>75</v>
@@ -4336,13 +4358,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="O3" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P3" s="44" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="Q3" s="44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R3" s="44">
         <v>0</v>
@@ -4351,21 +4373,21 @@
         <v>0</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B4" s="44">
         <v>2</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E4" s="44" t="s">
         <v>75</v>
@@ -4383,7 +4405,7 @@
         <v>72</v>
       </c>
       <c r="J4" s="44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K4" s="44" t="s">
         <v>75</v>
@@ -4399,13 +4421,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="O4" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P4" s="44" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="Q4" s="44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R4" s="44">
         <v>0</v>
@@ -4414,21 +4436,21 @@
         <v>0</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B5" s="44">
         <v>2</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D5" s="45" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E5" s="44" t="s">
         <v>75</v>
@@ -4446,7 +4468,7 @@
         <v>72</v>
       </c>
       <c r="J5" s="44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K5" s="44" t="s">
         <v>75</v>
@@ -4462,13 +4484,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="O5" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P5" s="44" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="Q5" s="44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R5" s="44">
         <v>0</v>
@@ -4477,21 +4499,21 @@
         <v>0</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B6" s="44">
         <v>2</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E6" s="44" t="s">
         <v>75</v>
@@ -4509,7 +4531,7 @@
         <v>72</v>
       </c>
       <c r="J6" s="44" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K6" s="44" t="s">
         <v>75</v>
@@ -4525,13 +4547,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="O6" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P6" s="44" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="Q6" s="44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R6" s="44">
         <v>0</v>
@@ -4540,7 +4562,7 @@
         <v>0</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -4551,10 +4573,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D7" s="45" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E7" s="44" t="s">
         <v>75</v>
@@ -4572,29 +4594,29 @@
         <v>72</v>
       </c>
       <c r="J7" s="48" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K7" s="44" t="s">
         <v>75</v>
       </c>
       <c r="L7" s="46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="M7" s="46" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="N7" s="44">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="O7" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P7" s="44" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="Q7" s="44" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="R7" s="44">
         <v>0</v>
@@ -4603,7 +4625,7 @@
         <v>0</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -4614,10 +4636,10 @@
         <v>3</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D8" s="44" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E8" s="44" t="s">
         <v>75</v>
@@ -4632,7 +4654,7 @@
         <v>1</v>
       </c>
       <c r="I8" s="44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J8" s="44" t="s">
         <v>77</v>
@@ -4650,13 +4672,13 @@
         <v>0</v>
       </c>
       <c r="O8" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P8" s="44">
         <v>0</v>
       </c>
       <c r="Q8" s="44" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="R8" s="44">
         <v>0</v>
@@ -4676,7 +4698,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D9" s="44" t="s">
         <v>76</v>
@@ -4712,13 +4734,13 @@
         <v>0</v>
       </c>
       <c r="O9" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P9" s="44">
         <v>0</v>
       </c>
       <c r="Q9" s="44" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="R9" s="44">
         <v>0</v>
@@ -4732,16 +4754,16 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B10" s="44">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D10" s="44" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" s="44" t="s">
         <v>75</v>
@@ -4752,14 +4774,14 @@
       <c r="G10" s="44">
         <v>0</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="44">
         <v>0</v>
       </c>
       <c r="I10" s="44" t="s">
         <v>72</v>
       </c>
       <c r="J10" s="44" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="K10" s="44" t="s">
         <v>75</v>
@@ -4770,40 +4792,40 @@
       <c r="M10" s="46">
         <v>0</v>
       </c>
-      <c r="N10" s="46">
-        <v>1.2</v>
+      <c r="N10" s="50" t="s">
+        <v>242</v>
       </c>
       <c r="O10" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P10" s="44">
         <v>0</v>
       </c>
       <c r="Q10" s="44" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="R10" s="44">
         <v>0</v>
       </c>
-      <c r="T10">
-        <v>0</v>
+      <c r="T10" t="s">
+        <v>82</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B11" s="44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D11" s="44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E11" s="44" t="s">
         <v>75</v>
@@ -4821,7 +4843,7 @@
         <v>72</v>
       </c>
       <c r="J11" s="44" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="K11" s="44" t="s">
         <v>75</v>
@@ -4832,88 +4854,26 @@
       <c r="M11" s="46">
         <v>0</v>
       </c>
-      <c r="N11" s="44" t="s">
-        <v>247</v>
+      <c r="N11" s="50" t="s">
+        <v>243</v>
       </c>
       <c r="O11" s="44" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P11" s="44">
         <v>0</v>
       </c>
       <c r="Q11" s="44" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="R11" s="44">
         <v>0</v>
       </c>
-      <c r="T11" t="s">
-        <v>84</v>
+      <c r="T11">
+        <v>0</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12" s="44">
-        <v>6</v>
-      </c>
-      <c r="C12" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="D12" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" s="44">
-        <v>0</v>
-      </c>
-      <c r="G12" s="44">
-        <v>0</v>
-      </c>
-      <c r="H12" s="44">
-        <v>0</v>
-      </c>
-      <c r="I12" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="K12" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="L12" s="44">
-        <v>0</v>
-      </c>
-      <c r="M12" s="46">
-        <v>0</v>
-      </c>
-      <c r="N12" s="44" t="s">
-        <v>248</v>
-      </c>
-      <c r="O12" s="44" t="s">
-        <v>176</v>
-      </c>
-      <c r="P12" s="44">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="R12" s="44">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -4926,10 +4886,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70AAB0C4-AECD-43D0-BAFA-6C4220D77958}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="D9" sqref="D9:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4986,7 +4946,7 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2">
         <v>1E-3</v>
@@ -5024,7 +4984,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="20" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B3">
         <v>1E-3</v>
@@ -5062,7 +5022,7 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="20" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B4">
         <v>1E-3</v>
@@ -5100,7 +5060,7 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="20" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B5">
         <v>1E-3</v>
@@ -5138,7 +5098,7 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B6">
         <v>1E-3</v>
@@ -5290,7 +5250,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="19" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -5328,7 +5288,7 @@
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="19" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -5361,44 +5321,6 @@
         <v>67</v>
       </c>
       <c r="L11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="A12" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="29">
-        <v>1E-10</v>
-      </c>
-      <c r="G12" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12">
-        <v>1000</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.6</v>
-      </c>
-      <c r="J12">
-        <v>10</v>
-      </c>
-      <c r="K12" t="s">
-        <v>67</v>
-      </c>
-      <c r="L12" t="s">
         <v>64</v>
       </c>
     </row>
@@ -5415,7 +5337,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R19" sqref="R19"/>
+      <selection pane="topRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -5436,22 +5358,22 @@
         <v>6</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C1" s="34" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E1" s="34" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="H1" s="34" t="s">
         <v>45</v>
@@ -5463,10 +5385,10 @@
         <v>54</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="L1" s="20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="M1" s="23" t="s">
         <v>19</v>
@@ -5475,12 +5397,12 @@
         <v>20</v>
       </c>
       <c r="O1" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="35" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B2" s="14">
         <v>0</v>
@@ -5527,13 +5449,13 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="34" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B3" s="9">
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D3" s="5">
         <v>0</v>
@@ -5574,7 +5496,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="34" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
@@ -5583,7 +5505,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -5621,19 +5543,19 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="B5" s="9">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>124</v>
       </c>
       <c r="F5" s="5">
         <v>0</v>
@@ -5668,22 +5590,22 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="B6" s="9">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-      <c r="E6" s="9">
-        <v>0</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>125</v>
       </c>
       <c r="G6" s="5">
         <v>0</v>
@@ -5715,25 +5637,25 @@
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0</v>
+      </c>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="B7" s="9">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9">
-        <v>0</v>
-      </c>
-      <c r="F7" s="9">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>126</v>
       </c>
       <c r="H7" s="5">
         <v>0</v>
@@ -5783,7 +5705,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="I8" s="6" t="s">
         <v>23</v>
@@ -5833,7 +5755,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="J9" s="9">
         <v>0</v>
@@ -5841,8 +5763,8 @@
       <c r="K9" s="9">
         <v>0</v>
       </c>
-      <c r="L9" s="9">
-        <v>0</v>
+      <c r="L9" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="M9" s="9">
         <v>0</v>
@@ -5883,7 +5805,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>23</v>
@@ -5903,7 +5825,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="A11" s="22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B11" s="9">
         <v>0</v>
@@ -5950,7 +5872,7 @@
     </row>
     <row r="12" spans="1:15">
       <c r="A12" s="22" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B12" s="9">
         <v>0</v>
@@ -6091,7 +6013,7 @@
     </row>
     <row r="15" spans="1:15">
       <c r="A15" s="23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
@@ -6147,7 +6069,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B8 B9:O15 C4:C7 C8:G8 C2:O2 D5:D7 D3:H3 E4 E6:E7 F4:F5 F7 G4:G6 H4:H7 I3:O8">
+  <conditionalFormatting sqref="B3:B8 C4:C7 C8:G8 C2:O2 D5:D7 D3:H3 E4 E6:E7 F4:F5 F7 G4:G6 H4:H7 I3:O8 B9:O15">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -6168,8 +6090,8 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2:A6"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -6190,7 +6112,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -6216,10 +6138,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C2" s="33">
         <v>0</v>
@@ -6234,21 +6156,21 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C3" s="33">
         <v>0</v>
@@ -6263,21 +6185,21 @@
         <v>0</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C4" s="33">
         <v>0</v>
@@ -6292,21 +6214,21 @@
         <v>0</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C5" s="33">
         <v>0</v>
@@ -6321,21 +6243,21 @@
         <v>0</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C6" s="33">
         <v>0</v>
@@ -6350,18 +6272,18 @@
         <v>0</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B7" s="33">
         <v>0</v>
@@ -6373,19 +6295,19 @@
         <v>46</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G7" s="40">
         <v>0</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="I7" s="40" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6413,7 +6335,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6428,51 +6350,51 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="K1" t="s">
         <v>140</v>
       </c>
-      <c r="G1" t="s">
+      <c r="L1" t="s">
         <v>141</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>142</v>
       </c>
-      <c r="I1" t="s">
+      <c r="N1" t="s">
         <v>143</v>
-      </c>
-      <c r="J1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L1" t="s">
-        <v>146</v>
-      </c>
-      <c r="M1" t="s">
-        <v>147</v>
-      </c>
-      <c r="N1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="25" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C2" s="26" t="s">
         <v>71</v>
@@ -6502,10 +6424,10 @@
         <v>0.5</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M2" s="28">
         <v>100</v>
@@ -6516,13 +6438,13 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="25" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D3" s="13">
         <v>0.95</v>
@@ -6549,10 +6471,10 @@
         <v>0.5</v>
       </c>
       <c r="K3" s="28" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="L3" s="28" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M3" s="28">
         <v>100</v>
@@ -6563,13 +6485,13 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="25" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D4" s="13">
         <v>0.95</v>
@@ -6596,10 +6518,10 @@
         <v>0.5</v>
       </c>
       <c r="K4" s="28" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="M4" s="28">
         <v>100</v>
@@ -6617,8 +6539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFEA29F-1D3A-4383-97E1-D31836BA3887}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H22" sqref="H21:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -6700,26 +6622,26 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6727,23 +6649,23 @@
         <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -6766,10 +6688,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -6777,123 +6699,123 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" t="s">
         <v>153</v>
-      </c>
-      <c r="C7" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B11" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C12" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -6922,10 +6844,10 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -6933,10 +6855,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>74</v>
@@ -6945,7 +6867,7 @@
         <v>28</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H3" s="9" t="s">
         <v>55</v>
@@ -6964,28 +6886,28 @@
         <v>8</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H4" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -6993,28 +6915,28 @@
         <v>7</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -7022,28 +6944,28 @@
         <v>9</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -7051,28 +6973,28 @@
         <v>10</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H7" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I7" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J7" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -7080,28 +7002,28 @@
         <v>25</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -7109,28 +7031,28 @@
         <v>45</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -7138,28 +7060,28 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C10" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -7167,28 +7089,28 @@
         <v>54</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I11" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -7196,28 +7118,28 @@
         <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D12" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -7225,28 +7147,28 @@
         <v>51</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -7254,28 +7176,28 @@
         <v>52</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:12">

</xml_diff>

<commit_message>
updated prices and added solve_model function
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v2.xlsx
+++ b/excel files/propionate_case_study_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D04EBE40-6266-43E0-8291-651E512C1588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156CBF11-18C0-4F52-A8ED-44A22C08696A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="parameter_abbr" sheetId="24" r:id="rId8"/>
     <sheet name="references" sheetId="19" r:id="rId9"/>
     <sheet name="price_list" sheetId="26" r:id="rId10"/>
-    <sheet name="final_conc_reactors" sheetId="27" r:id="rId11"/>
+    <sheet name="price_list_sigma" sheetId="28" r:id="rId11"/>
+    <sheet name="final_conc_reactors" sheetId="27" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="258">
   <si>
     <t>components</t>
   </si>
@@ -811,12 +812,54 @@
   <si>
     <t>Distillation_3.json</t>
   </si>
+  <si>
+    <t>https://shuowanchemical.en.made-in-china.com/product/XQoUxvSJhVcb/China-99-5-CAS-79-09-4-Propionic-Acid-for-Food-Preservatives.html</t>
+  </si>
+  <si>
+    <t>https://sunwisechem.en.made-in-china.com/product/lZTakcfLhyUb/China-Colorless-Price-90-CH3cooh-CAS-No-64-19-7-Industrial-Grade-Acetic-Acid.html</t>
+  </si>
+  <si>
+    <t>USD/kg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://shuowanchemical.en.made-in-china.com/product/XQoUxvSJhVcb/China-99-5-CAS-79-09-4-Propionic-Acid-for-Food-Preservatives.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://yaoshengcompany.en.made-in-china.com/product/RZwtMgVCEqUT/China-Food-Grade-Glucose-Dextrose-Monohydrate-Dextrose-Anhydrous.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://sunwisechem.en.made-in-china.com/product/lZTakcfLhyUb/China-Colorless-Price-90-CH3cooh-CAS-No-64-19-7-Industrial-Grade-Acetic-Acid.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hbsyplastic.en.made-in-china.com/product/VZFAzMXKykrq/China-99-5-Pure-Glycerol-with-Competitive-Price-Refined-Glycerol-Glycerol-Glycerine.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://qddoeast.en.made-in-china.com/product/EKXmIwiTszrt/China-Food-Additive-Corn-Fiber-Organic-Resistant-Dextrin-Powder.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hairunkun.en.made-in-china.com/product/ZFeAPoVdStry/China-The-Factory-Supplies-The-Most-Competitive-Food-Grade-Stachyose.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.made-in-china.com/productdirectory.do?subaction=hunt&amp;style=b&amp;mode=and&amp;code=0&amp;comProvince=nolimit&amp;order=0&amp;isOpenCorrection=1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://luzhoubiochem.en.made-in-china.com/product/CKvErNtOXxpL/China-Hot-Sale-Fructose-Syrup-Fructose-42-55-Food-Grade.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://luzhoubiochem.en.made-in-china.com/product/FXNmbhUKfEYB/China-Beer-Food-Additives-Maltose-Syrup.html </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://hbsyplastic.en.made-in-china.com/product/PFjtVDIcZqYU/China-2022-Hot-Selling-Food-Grade-High-Purity-Powder-Sucrose-99-.html  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://ubchembio.en.made-in-china.com/product/iwzfCWIcnhVG/China-Wholesale-Price-Food-Grade-Liquid-L-Lactic-Acid-80-CAS-50-21-5.html </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,6 +948,13 @@
       <color rgb="FF333333"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFFF0000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1081,7 +1131,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1194,6 +1244,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3704,8 +3757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -3757,7 +3810,7 @@
         <v>208</v>
       </c>
       <c r="C2" s="4">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
@@ -3792,7 +3845,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>50.5</v>
+        <v>0.75</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>17</v>
@@ -3818,7 +3871,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>78.5</v>
+        <v>1.5</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>16</v>
@@ -3846,10 +3899,214 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5896565C-0CFB-4158-9B0C-FB654BCEAE1A}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2">
+        <v>0.37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3">
+        <v>1.85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>246</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4">
+        <v>0.4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="B5">
+        <v>0.51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="B8">
+        <v>3.5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>246</v>
+      </c>
+      <c r="D8" s="42" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="B9">
+        <v>0.85</v>
+      </c>
+      <c r="C9" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="42" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="B10">
+        <v>0.45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="42" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="51" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11">
+        <v>1.25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>246</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="51" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12">
+        <v>0.75</v>
+      </c>
+      <c r="C12" t="s">
+        <v>246</v>
+      </c>
+      <c r="D12" s="42" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="43"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{291BDE3D-39D1-4A5F-8AE8-38D12FACEBEA}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{30E600D4-05E2-43D5-ADDD-73424F47F91D}"/>
+    <hyperlink ref="D12" r:id="rId3" xr:uid="{5506D572-E27E-4AFF-BA0F-006BFCB04704}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{AC8CF186-BAD9-4525-9887-B3A6409D1D52}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{6BCBEB49-53CD-4FB9-A741-B4B122942000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{092DD633-0AC1-4F6C-BAB1-C79B8883E3C5}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{C98486F0-077B-4740-8AF0-20CBA02E0195}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{7025CCBD-77ED-41A8-8A69-2D69E5C2183E}"/>
+    <hyperlink ref="D3" r:id="rId9" xr:uid="{664A5837-CF7C-409A-BE98-AFB718953232}"/>
+    <hyperlink ref="D2" r:id="rId10" xr:uid="{B031B00F-21F7-464A-B559-3CB7506D9BED}"/>
+    <hyperlink ref="D4" r:id="rId11" xr:uid="{042C6450-ED4A-4FAE-883C-F3B67CDCDACA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{975FC6AB-3E76-4672-B327-5D80D9EC35D9}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4011,7 +4268,9 @@
       <c r="D11" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="E11" s="43"/>
+      <c r="E11" s="43" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="30" t="s">
@@ -4026,7 +4285,9 @@
       <c r="D12" t="s">
         <v>213</v>
       </c>
-      <c r="E12" s="43"/>
+      <c r="E12" s="43" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="43"/>
@@ -4037,7 +4298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7C6831-8C7B-4CA3-B2A4-37C4E254EDCB}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -4159,7 +4420,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M14" sqref="M14"/>
+      <selection pane="topRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4889,7 +5150,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D11"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4967,13 +5228,13 @@
         <v>61</v>
       </c>
       <c r="H2">
-        <v>1000</v>
-      </c>
-      <c r="I2" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K2" t="s">
         <v>67</v>
@@ -5005,13 +5266,13 @@
         <v>61</v>
       </c>
       <c r="H3">
-        <v>1000</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
         <v>67</v>
@@ -5043,13 +5304,13 @@
         <v>61</v>
       </c>
       <c r="H4">
-        <v>1000</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K4" t="s">
         <v>67</v>
@@ -5081,13 +5342,13 @@
         <v>61</v>
       </c>
       <c r="H5">
-        <v>1000</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
       </c>
       <c r="J5">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
         <v>67</v>
@@ -5119,13 +5380,13 @@
         <v>61</v>
       </c>
       <c r="H6">
-        <v>1000</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
         <v>67</v>
@@ -5157,13 +5418,13 @@
         <v>61</v>
       </c>
       <c r="H7">
-        <v>1000</v>
-      </c>
-      <c r="I7" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K7" t="s">
         <v>67</v>
@@ -5195,13 +5456,13 @@
         <v>61</v>
       </c>
       <c r="H8">
-        <v>1000</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K8" t="s">
         <v>67</v>
@@ -5233,13 +5494,13 @@
         <v>61</v>
       </c>
       <c r="H9">
-        <v>1000</v>
-      </c>
-      <c r="I9" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
       </c>
       <c r="J9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K9" t="s">
         <v>67</v>
@@ -5271,13 +5532,13 @@
         <v>61</v>
       </c>
       <c r="H10">
-        <v>1000</v>
-      </c>
-      <c r="I10" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
       </c>
       <c r="J10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K10" t="s">
         <v>67</v>
@@ -5309,13 +5570,13 @@
         <v>61</v>
       </c>
       <c r="H11">
-        <v>1000</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.6</v>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K11" t="s">
         <v>67</v>
@@ -5335,7 +5596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BC952C-F64C-4F30-9DDA-924F82AF01AE}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="J17" sqref="J17"/>
     </sheetView>
@@ -6828,7 +7089,7 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
broken because of energy price, idk why
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v2.xlsx
+++ b/excel files/propionate_case_study_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6014E4BB-1788-4EBA-B95C-20AB6F29DC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D6C90C-F1F1-4437-960E-E1AE71CFF123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" tabRatio="683" activeTab="2" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="312">
   <si>
     <t>components</t>
   </si>
@@ -416,9 +416,6 @@
     <t>units</t>
   </si>
   <si>
-    <t>[0.95, 0.95, 0.95, 0] ; [0.05, 0.05, 0.05, 1]</t>
-  </si>
-  <si>
     <t>Dist1.json</t>
   </si>
   <si>
@@ -534,9 +531,6 @@
   </si>
   <si>
     <t>energy_consumption</t>
-  </si>
-  <si>
-    <t>kWh/kg</t>
   </si>
   <si>
     <t xml:space="preserve">DWA </t>
@@ -764,6 +758,12 @@
     <t>fed-batch (FFB, biomass contained in fibers)</t>
   </si>
   <si>
+    <t>Distillation_2.json</t>
+  </si>
+  <si>
+    <t>Distillation_3.json</t>
+  </si>
+  <si>
     <t>https://shuowanchemical.en.made-in-china.com/product/XQoUxvSJhVcb/China-99-5-CAS-79-09-4-Propionic-Acid-for-Food-Preservatives.html</t>
   </si>
   <si>
@@ -992,7 +992,16 @@
     <t>price_USD</t>
   </si>
   <si>
-    <t xml:space="preserve">Distillation_2.json </t>
+    <t>not considering the solvent seeing as in the model only 0.3 kg_solvent/h is being added ()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i.e. the solvent that is lost during the </t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 0] ; [0, 0, 0, 1]</t>
+  </si>
+  <si>
+    <t>kWh/(kg/h)</t>
   </si>
 </sst>
 </file>
@@ -1558,7 +1567,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4123,7 +4132,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -4138,7 +4147,7 @@
     <col min="8" max="8" width="7.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4178,7 +4187,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -4190,7 +4199,7 @@
         <v>265</v>
       </c>
       <c r="F2" s="33" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -4199,7 +4208,7 @@
         <v>60</v>
       </c>
       <c r="I2" s="33" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J2" s="4">
         <v>1</v>
@@ -4225,7 +4234,6 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <f>0.6</f>
         <v>0.6</v>
       </c>
       <c r="H3" t="s">
@@ -4258,7 +4266,6 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <f>2.25</f>
         <v>2.25</v>
       </c>
       <c r="H4" t="s">
@@ -4314,7 +4321,7 @@
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E1" t="s">
         <v>122</v>
@@ -4325,7 +4332,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B2">
         <v>0.37</v>
@@ -4346,7 +4353,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3">
         <v>1.85</v>
@@ -4367,7 +4374,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4">
         <v>0.4</v>
@@ -4388,7 +4395,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B5">
         <v>0.51</v>
@@ -4409,7 +4416,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4430,7 +4437,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -4451,7 +4458,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B8">
         <v>3.5</v>
@@ -4472,7 +4479,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9">
         <v>0.85</v>
@@ -4493,7 +4500,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10">
         <v>0.45</v>
@@ -4514,7 +4521,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="46" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B11">
         <f>2.25 *1.1</f>
@@ -4536,7 +4543,7 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="46" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B12">
         <f>0.6*1.1</f>
@@ -4601,7 +4608,7 @@
         <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -4612,7 +4619,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="25" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B2">
         <v>222</v>
@@ -4621,12 +4628,12 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3">
         <v>85.8</v>
@@ -4635,12 +4642,12 @@
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B4">
         <v>64.3</v>
@@ -4649,12 +4656,12 @@
         <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B5">
         <v>74.8</v>
@@ -4663,12 +4670,12 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6">
         <v>61.1</v>
@@ -4677,12 +4684,12 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="25" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B7">
         <v>381</v>
@@ -4691,12 +4698,12 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B8">
         <v>53.6</v>
@@ -4705,12 +4712,12 @@
         <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="25" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B9">
         <v>53.3</v>
@@ -4719,12 +4726,12 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10">
         <v>52.3</v>
@@ -4733,12 +4740,12 @@
         <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="25" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B11">
         <v>78.5</v>
@@ -4747,7 +4754,7 @@
         <v>60</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E11" s="38" t="s">
         <v>232</v>
@@ -4755,7 +4762,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="25" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B12">
         <v>50.5</v>
@@ -4764,7 +4771,7 @@
         <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E12" s="38" t="s">
         <v>233</v>
@@ -4797,27 +4804,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B2" s="4">
         <v>37</v>
@@ -4826,21 +4833,21 @@
         <v>69</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C3" t="s">
         <v>69</v>
@@ -4848,31 +4855,31 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B7" s="4">
         <v>71</v>
@@ -4881,10 +4888,10 @@
         <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -4900,8 +4907,8 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P14" sqref="P14"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4919,7 +4926,7 @@
     <col min="12" max="12" width="31.6328125" customWidth="1"/>
     <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.08984375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18.54296875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11.7265625" bestFit="1" customWidth="1"/>
@@ -4980,7 +4987,7 @@
         <v>72</v>
       </c>
       <c r="Q1" s="42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="R1" s="42" t="s">
         <v>59</v>
@@ -5003,7 +5010,7 @@
         <v>119</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E2" s="39" t="s">
         <v>74</v>
@@ -5027,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="M2" s="39" t="s">
         <v>101</v>
@@ -5036,7 +5043,7 @@
         <v>74</v>
       </c>
       <c r="O2" s="69" t="s">
-        <v>123</v>
+        <v>310</v>
       </c>
       <c r="P2" s="39">
         <v>0</v>
@@ -5046,7 +5053,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R2" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -5066,7 +5073,7 @@
         <v>119</v>
       </c>
       <c r="D3" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E3" s="39" t="s">
         <v>74</v>
@@ -5090,7 +5097,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M3" s="39" t="s">
         <v>101</v>
@@ -5099,7 +5106,7 @@
         <v>74</v>
       </c>
       <c r="O3" s="69" t="s">
-        <v>123</v>
+        <v>310</v>
       </c>
       <c r="P3" s="39">
         <v>0</v>
@@ -5109,7 +5116,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R3" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -5129,7 +5136,7 @@
         <v>119</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E4" s="39" t="s">
         <v>74</v>
@@ -5153,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M4" s="39" t="s">
         <v>101</v>
@@ -5162,7 +5169,7 @@
         <v>74</v>
       </c>
       <c r="O4" s="69" t="s">
-        <v>123</v>
+        <v>310</v>
       </c>
       <c r="P4" s="39">
         <v>0</v>
@@ -5172,7 +5179,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R4" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -5192,7 +5199,7 @@
         <v>119</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E5" s="39" t="s">
         <v>74</v>
@@ -5216,7 +5223,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="M5" s="39" t="s">
         <v>101</v>
@@ -5225,7 +5232,7 @@
         <v>74</v>
       </c>
       <c r="O5" s="69" t="s">
-        <v>123</v>
+        <v>310</v>
       </c>
       <c r="P5" s="39">
         <v>0</v>
@@ -5235,7 +5242,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R5" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -5255,7 +5262,7 @@
         <v>119</v>
       </c>
       <c r="D6" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E6" s="39" t="s">
         <v>74</v>
@@ -5279,7 +5286,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M6" s="39" t="s">
         <v>101</v>
@@ -5288,7 +5295,7 @@
         <v>74</v>
       </c>
       <c r="O6" s="69" t="s">
-        <v>123</v>
+        <v>310</v>
       </c>
       <c r="P6" s="39">
         <v>0</v>
@@ -5298,7 +5305,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R6" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -5318,7 +5325,7 @@
         <v>119</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E7" s="39" t="s">
         <v>74</v>
@@ -5342,7 +5349,7 @@
         <v>120</v>
       </c>
       <c r="L7" s="39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M7" s="43" t="s">
         <v>101</v>
@@ -5351,7 +5358,7 @@
         <v>74</v>
       </c>
       <c r="O7" s="69" t="s">
-        <v>123</v>
+        <v>310</v>
       </c>
       <c r="P7" s="39">
         <v>0</v>
@@ -5361,7 +5368,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R7" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -5420,10 +5427,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="78">
-        <v>5.2994419171786343E-2</v>
+        <v>0.113</v>
       </c>
       <c r="R8" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -5481,11 +5488,11 @@
       <c r="P9" s="39">
         <v>0</v>
       </c>
-      <c r="Q9" s="79" t="s">
-        <v>308</v>
+      <c r="Q9" s="45" t="s">
+        <v>230</v>
       </c>
       <c r="R9" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V9" t="s">
         <v>81</v>
@@ -5543,11 +5550,11 @@
       <c r="P10" s="39">
         <v>0</v>
       </c>
-      <c r="Q10" s="45">
-        <v>0.6</v>
+      <c r="Q10" s="45" t="s">
+        <v>231</v>
       </c>
       <c r="R10" s="39" t="s">
-        <v>163</v>
+        <v>311</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -5569,7 +5576,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -5635,7 +5642,7 @@
       <c r="C2" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="36">
+      <c r="D2" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E2" s="53" t="s">
@@ -5673,7 +5680,7 @@
       <c r="C3" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E3" s="57" t="s">
@@ -5711,7 +5718,7 @@
       <c r="C4" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E4" s="57" t="s">
@@ -5749,7 +5756,7 @@
       <c r="C5" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E5" s="57" t="s">
@@ -5787,7 +5794,7 @@
       <c r="C6" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E6" s="57" t="s">
@@ -5825,7 +5832,7 @@
       <c r="C7" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E7" s="61" t="s">
@@ -5863,7 +5870,7 @@
       <c r="C8" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="36">
+      <c r="D8" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E8" s="53" t="s">
@@ -5901,7 +5908,7 @@
       <c r="C9" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E9" s="57" t="s">
@@ -5939,7 +5946,7 @@
       <c r="C10" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="62">
+      <c r="D10" s="79">
         <v>2.2000000000000002</v>
       </c>
       <c r="E10" s="61" t="s">
@@ -6001,7 +6008,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>106</v>
@@ -6042,7 +6049,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="30" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B2" s="12">
         <v>0</v>
@@ -6623,7 +6630,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 C3 E5 F6 G7 H8">
+  <conditionalFormatting sqref="C3 D4 E5 F6 G7 H8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6666,7 +6673,7 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>30</v>
@@ -6692,10 +6699,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C2" s="28">
         <v>0</v>
@@ -6713,18 +6720,18 @@
         <v>100</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C3" s="28">
         <v>0</v>
@@ -6742,18 +6749,18 @@
         <v>100</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C4" s="28">
         <v>0</v>
@@ -6771,18 +6778,18 @@
         <v>100</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B5" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C5" s="28">
         <v>0</v>
@@ -6800,18 +6807,18 @@
         <v>100</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C6" s="28">
         <v>0</v>
@@ -6829,15 +6836,15 @@
         <v>100</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B7" s="28">
         <v>0</v>
@@ -6849,19 +6856,19 @@
         <v>46</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G7" s="35">
         <v>0</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="I7" s="35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -6889,7 +6896,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6904,51 +6911,51 @@
         <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>127</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>128</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>129</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>130</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>131</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>132</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>133</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>134</v>
-      </c>
-      <c r="N1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>70</v>
@@ -6978,10 +6985,10 @@
         <v>0.5</v>
       </c>
       <c r="K2" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L2" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M2" s="24">
         <v>100</v>
@@ -6992,10 +6999,10 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>95</v>
@@ -7025,10 +7032,10 @@
         <v>0.5</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M3" s="24">
         <v>100</v>
@@ -7039,13 +7046,13 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>158</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>159</v>
       </c>
       <c r="D4" s="11">
         <v>0.95</v>
@@ -7072,10 +7079,10 @@
         <v>0.5</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L4" s="24" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M4" s="24">
         <v>100</v>
@@ -7094,7 +7101,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -7216,10 +7223,10 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -7242,10 +7249,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" t="s">
         <v>160</v>
-      </c>
-      <c r="B1" t="s">
-        <v>161</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -7253,10 +7260,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
         <v>120</v>
@@ -7264,10 +7271,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C3" t="s">
         <v>120</v>
@@ -7275,10 +7282,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" t="s">
         <v>121</v>
@@ -7286,10 +7293,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" t="s">
         <v>121</v>
@@ -7297,10 +7304,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C6" t="s">
         <v>121</v>
@@ -7308,68 +7315,68 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -7381,8 +7388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE819A9C-4E64-4D0F-8F31-2F1BF4DCFD79}">
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Q35" sqref="Q35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7424,10 +7431,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>73</v>
@@ -7475,19 +7482,19 @@
         <v>8</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G4" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H4" s="76" t="s">
         <v>288</v>
@@ -7535,19 +7542,19 @@
         <v>7</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G5" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H5" s="76" t="s">
         <v>288</v>
@@ -7594,19 +7601,19 @@
         <v>9</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G6" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H6" s="76" t="s">
         <v>288</v>
@@ -7641,19 +7648,19 @@
         <v>10</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G7" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H7" s="76" t="s">
         <v>288</v>
@@ -7667,19 +7674,19 @@
         <v>25</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G8" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H8" s="76" t="s">
         <v>288</v>
@@ -7707,8 +7714,8 @@
         <v>304</v>
       </c>
       <c r="Y8" s="74">
-        <f xml:space="preserve"> Y4/(Y5 + Y6)</f>
-        <v>5.2994419171786343E-2</v>
+        <f xml:space="preserve"> Y4/(Y5 )</f>
+        <v>0.1134538152610442</v>
       </c>
       <c r="Z8" t="s">
         <v>305</v>
@@ -7719,19 +7726,19 @@
         <v>45</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>166</v>
-      </c>
       <c r="G9" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H9" s="76" t="s">
         <v>288</v>
@@ -7747,6 +7754,9 @@
       </c>
       <c r="R9" s="1" t="s">
         <v>245</v>
+      </c>
+      <c r="X9" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -7754,16 +7764,16 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G10" s="20" t="s">
         <v>287</v>
@@ -7782,6 +7792,9 @@
       </c>
       <c r="R10" t="s">
         <v>272</v>
+      </c>
+      <c r="X10" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -7792,16 +7805,16 @@
         <v>285</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>286</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G11" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H11" s="76" t="s">
         <v>288</v>
@@ -7824,19 +7837,19 @@
         <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D12" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G12" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H12" s="76" t="s">
         <v>288</v>
@@ -7859,19 +7872,19 @@
         <v>51</v>
       </c>
       <c r="B13" s="27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G13" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H13" s="76" t="s">
         <v>288</v>
@@ -7894,19 +7907,19 @@
         <v>52</v>
       </c>
       <c r="B14" s="27" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G14" s="75" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="H14" s="76" t="s">
         <v>288</v>

</xml_diff>

<commit_message>
adding small details (deleet stachyose e.g.)
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v2.xlsx
+++ b/excel files/propionate_case_study_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79750BA-8988-4899-A494-EDA7677A0064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C203BE-6357-4C1F-85F6-BCD6B0E593A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="321">
   <si>
     <t>components</t>
   </si>
@@ -1005,6 +1005,30 @@
   </si>
   <si>
     <t>kg/kgFeed</t>
+  </si>
+  <si>
+    <t>loss of solvent in water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">solubity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">loss solvent </t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?q=hexyl+acetate+solubility+in+water&amp;rlz=1C1QPHC_nlBE987BE987&amp;oq=solubility+hexyl+acetat&amp;aqs=chrome.2.69i57j0i22i30l2j0i8i13i15i30j0i390i650l5.8117j0j7&amp;sourceid=chrome&amp;ie=UTF-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">loss per kg entering </t>
+  </si>
+  <si>
+    <t>kgSolvent/kgFeed</t>
+  </si>
+  <si>
+    <t>g/h</t>
   </si>
 </sst>
 </file>
@@ -1063,12 +1087,6 @@
       <color rgb="FF008000"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1130,6 +1148,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FFFFC000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="15">
@@ -1387,7 +1412,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1449,9 +1474,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1473,12 +1495,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1487,14 +1509,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1505,7 +1527,7 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1538,19 +1560,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1561,6 +1583,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3781,16 +3806,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>86784</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>36969</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>72876</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>428553</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>168127</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3813,8 +3838,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="24809450" y="3314700"/>
-          <a:ext cx="9047619" cy="1190476"/>
+          <a:off x="20478750" y="3166534"/>
+          <a:ext cx="9075136" cy="1160843"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4157,7 +4182,7 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="46" t="s">
         <v>59</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -4166,7 +4191,7 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="46" t="s">
         <v>120</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -4192,7 +4217,7 @@
       <c r="E2" t="s">
         <v>263</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>195</v>
       </c>
       <c r="G2" s="4">
@@ -4201,7 +4226,7 @@
       <c r="H2" t="s">
         <v>60</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="32" t="s">
         <v>195</v>
       </c>
       <c r="J2" s="4">
@@ -4293,8 +4318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5896565C-0CFB-4158-9B0C-FB654BCEAE1A}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A10" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4334,19 +4359,19 @@
       <c r="C2" t="s">
         <v>232</v>
       </c>
-      <c r="D2" s="70">
+      <c r="D2" s="69">
         <f>B2*1/1.1</f>
         <v>0.33636363636363631</v>
       </c>
       <c r="E2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="36" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="77" t="s">
         <v>184</v>
       </c>
       <c r="B3">
@@ -4355,14 +4380,14 @@
       <c r="C3" t="s">
         <v>232</v>
       </c>
-      <c r="D3" s="70">
+      <c r="D3" s="69">
         <f t="shared" ref="D3:D12" si="0">B3*1/1.1</f>
         <v>1.6818181818181817</v>
       </c>
       <c r="E3" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="36" t="s">
         <v>240</v>
       </c>
     </row>
@@ -4376,14 +4401,14 @@
       <c r="C4" t="s">
         <v>232</v>
       </c>
-      <c r="D4" s="70">
+      <c r="D4" s="69">
         <f t="shared" si="0"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="E4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="36" t="s">
         <v>241</v>
       </c>
     </row>
@@ -4397,14 +4422,14 @@
       <c r="C5" t="s">
         <v>232</v>
       </c>
-      <c r="D5" s="70">
+      <c r="D5" s="69">
         <f t="shared" si="0"/>
         <v>0.46363636363636362</v>
       </c>
       <c r="E5" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="36" t="s">
         <v>238</v>
       </c>
     </row>
@@ -4418,19 +4443,19 @@
       <c r="C6" t="s">
         <v>232</v>
       </c>
-      <c r="D6" s="70">
+      <c r="D6" s="69">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
       <c r="E6" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="36" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="77" t="s">
         <v>188</v>
       </c>
       <c r="B7">
@@ -4439,14 +4464,14 @@
       <c r="C7" t="s">
         <v>232</v>
       </c>
-      <c r="D7" s="70">
+      <c r="D7" s="69">
         <f t="shared" si="0"/>
         <v>5.4545454545454541</v>
       </c>
       <c r="E7" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="36" t="s">
         <v>236</v>
       </c>
     </row>
@@ -4460,14 +4485,14 @@
       <c r="C8" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="70">
+      <c r="D8" s="69">
         <f t="shared" si="0"/>
         <v>3.1818181818181817</v>
       </c>
       <c r="E8" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="36" t="s">
         <v>235</v>
       </c>
     </row>
@@ -4481,14 +4506,14 @@
       <c r="C9" t="s">
         <v>232</v>
       </c>
-      <c r="D9" s="70">
+      <c r="D9" s="69">
         <f t="shared" si="0"/>
         <v>0.7727272727272726</v>
       </c>
       <c r="E9" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="36" t="s">
         <v>234</v>
       </c>
     </row>
@@ -4502,19 +4527,19 @@
       <c r="C10" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="70">
+      <c r="D10" s="69">
         <f t="shared" si="0"/>
         <v>0.40909090909090906</v>
       </c>
       <c r="E10" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="46" t="s">
+      <c r="A11" s="45" t="s">
         <v>192</v>
       </c>
       <c r="B11">
@@ -4524,19 +4549,19 @@
       <c r="C11" t="s">
         <v>232</v>
       </c>
-      <c r="D11" s="70">
+      <c r="D11" s="69">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
       <c r="E11" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="36" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="46" t="s">
+      <c r="A12" s="45" t="s">
         <v>193</v>
       </c>
       <c r="B12">
@@ -4546,19 +4571,19 @@
       <c r="C12" t="s">
         <v>232</v>
       </c>
-      <c r="D12" s="70">
+      <c r="D12" s="69">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
       <c r="E12" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="36" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="38"/>
+      <c r="A14" s="37"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4747,10 +4772,10 @@
       <c r="C11" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="37" t="s">
         <v>230</v>
       </c>
     </row>
@@ -4767,12 +4792,12 @@
       <c r="D12" t="s">
         <v>199</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="37" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="38"/>
+      <c r="A14" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4826,10 +4851,10 @@
       <c r="C2" t="s">
         <v>67</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="E2" s="43" t="s">
         <v>219</v>
       </c>
       <c r="F2" t="s">
@@ -4901,8 +4926,8 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H18" sqref="H18"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4935,55 +4960,55 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="41" t="s">
         <v>311</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="42" t="s">
+      <c r="N1" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="O1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="Q1" s="42" t="s">
+      <c r="Q1" s="41" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="42" t="s">
+      <c r="R1" s="41" t="s">
         <v>59</v>
       </c>
       <c r="V1" s="14" t="s">
@@ -4997,56 +5022,56 @@
       <c r="A2" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="39">
+      <c r="B2" s="38">
         <v>2</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="D2" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="39">
-        <v>0</v>
-      </c>
-      <c r="G2" s="39">
-        <v>0</v>
-      </c>
-      <c r="H2" s="39">
-        <v>0</v>
-      </c>
-      <c r="I2" s="39" t="s">
+      <c r="F2" s="38">
+        <v>0</v>
+      </c>
+      <c r="G2" s="38">
+        <v>0</v>
+      </c>
+      <c r="H2" s="38">
+        <v>0</v>
+      </c>
+      <c r="I2" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="41">
-        <v>0</v>
-      </c>
-      <c r="K2" s="39">
-        <v>0</v>
-      </c>
-      <c r="L2" s="39" t="s">
+      <c r="J2" s="40">
+        <v>0</v>
+      </c>
+      <c r="K2" s="38">
+        <v>0</v>
+      </c>
+      <c r="L2" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="66" t="s">
+      <c r="O2" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="P2" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="39">
+      <c r="P2" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="38">
         <f xml:space="preserve"> 0.5*0.001</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="R2" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V2">
@@ -5060,56 +5085,56 @@
       <c r="A3" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="39">
+      <c r="B3" s="38">
         <v>2</v>
       </c>
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="39">
-        <v>0</v>
-      </c>
-      <c r="G3" s="39">
-        <v>0</v>
-      </c>
-      <c r="H3" s="39">
-        <v>0</v>
-      </c>
-      <c r="I3" s="39" t="s">
+      <c r="F3" s="38">
+        <v>0</v>
+      </c>
+      <c r="G3" s="38">
+        <v>0</v>
+      </c>
+      <c r="H3" s="38">
+        <v>0</v>
+      </c>
+      <c r="I3" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="39">
-        <v>0</v>
-      </c>
-      <c r="K3" s="39">
-        <v>0</v>
-      </c>
-      <c r="L3" s="39" t="s">
+      <c r="J3" s="38">
+        <v>0</v>
+      </c>
+      <c r="K3" s="38">
+        <v>0</v>
+      </c>
+      <c r="L3" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="N3" s="39" t="s">
+      <c r="N3" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O3" s="66" t="s">
+      <c r="O3" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="P3" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="39">
+      <c r="P3" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="38">
         <f t="shared" ref="Q3:Q7" si="0" xml:space="preserve"> 0.5*0.001</f>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="R3" s="39" t="s">
+      <c r="R3" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V3">
@@ -5123,56 +5148,56 @@
       <c r="A4" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="38">
         <v>2</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="40" t="s">
+      <c r="D4" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="39">
-        <v>0</v>
-      </c>
-      <c r="G4" s="39">
-        <v>0</v>
-      </c>
-      <c r="H4" s="39">
-        <v>0</v>
-      </c>
-      <c r="I4" s="39" t="s">
+      <c r="F4" s="38">
+        <v>0</v>
+      </c>
+      <c r="G4" s="38">
+        <v>0</v>
+      </c>
+      <c r="H4" s="38">
+        <v>0</v>
+      </c>
+      <c r="I4" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="39">
-        <v>0</v>
-      </c>
-      <c r="K4" s="39">
-        <v>0</v>
-      </c>
-      <c r="L4" s="39" t="s">
+      <c r="J4" s="38">
+        <v>0</v>
+      </c>
+      <c r="K4" s="38">
+        <v>0</v>
+      </c>
+      <c r="L4" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="N4" s="39" t="s">
+      <c r="N4" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="66" t="s">
+      <c r="O4" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="P4" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="39">
+      <c r="P4" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="38">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="R4" s="39" t="s">
+      <c r="R4" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V4">
@@ -5186,56 +5211,56 @@
       <c r="A5" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="38">
         <v>2</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D5" s="40" t="s">
+      <c r="D5" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="39">
-        <v>0</v>
-      </c>
-      <c r="G5" s="39">
-        <v>0</v>
-      </c>
-      <c r="H5" s="39">
-        <v>0</v>
-      </c>
-      <c r="I5" s="39" t="s">
+      <c r="F5" s="38">
+        <v>0</v>
+      </c>
+      <c r="G5" s="38">
+        <v>0</v>
+      </c>
+      <c r="H5" s="38">
+        <v>0</v>
+      </c>
+      <c r="I5" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="39">
-        <v>0</v>
-      </c>
-      <c r="K5" s="39">
-        <v>0</v>
-      </c>
-      <c r="L5" s="39" t="s">
+      <c r="J5" s="38">
+        <v>0</v>
+      </c>
+      <c r="K5" s="38">
+        <v>0</v>
+      </c>
+      <c r="L5" s="38" t="s">
         <v>181</v>
       </c>
-      <c r="M5" s="39" t="s">
+      <c r="M5" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="N5" s="39" t="s">
+      <c r="N5" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O5" s="66" t="s">
+      <c r="O5" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="P5" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="39">
+      <c r="P5" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="38">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="R5" s="39" t="s">
+      <c r="R5" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V5">
@@ -5249,56 +5274,56 @@
       <c r="A6" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="38">
         <v>2</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D6" s="40" t="s">
+      <c r="D6" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F6" s="39">
-        <v>0</v>
-      </c>
-      <c r="G6" s="39">
-        <v>0</v>
-      </c>
-      <c r="H6" s="39">
-        <v>0</v>
-      </c>
-      <c r="I6" s="39" t="s">
+      <c r="F6" s="38">
+        <v>0</v>
+      </c>
+      <c r="G6" s="38">
+        <v>0</v>
+      </c>
+      <c r="H6" s="38">
+        <v>0</v>
+      </c>
+      <c r="I6" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J6" s="39">
-        <v>0</v>
-      </c>
-      <c r="K6" s="39">
-        <v>0</v>
-      </c>
-      <c r="L6" s="39" t="s">
+      <c r="J6" s="38">
+        <v>0</v>
+      </c>
+      <c r="K6" s="38">
+        <v>0</v>
+      </c>
+      <c r="L6" s="38" t="s">
         <v>182</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="38" t="s">
         <v>99</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="N6" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O6" s="66" t="s">
+      <c r="O6" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="P6" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="39">
+      <c r="P6" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="38">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="R6" s="39" t="s">
+      <c r="R6" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V6">
@@ -5312,56 +5337,56 @@
       <c r="A7" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="38">
         <v>2</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E7" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="41">
-        <v>0</v>
-      </c>
-      <c r="G7" s="39">
-        <v>0</v>
-      </c>
-      <c r="H7" s="39">
-        <v>0</v>
-      </c>
-      <c r="I7" s="39" t="s">
+      <c r="F7" s="40">
+        <v>0</v>
+      </c>
+      <c r="G7" s="38">
+        <v>0</v>
+      </c>
+      <c r="H7" s="38">
+        <v>0</v>
+      </c>
+      <c r="I7" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="K7" s="41" t="s">
+      <c r="K7" s="40" t="s">
         <v>118</v>
       </c>
-      <c r="L7" s="39" t="s">
+      <c r="L7" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="M7" s="43" t="s">
+      <c r="M7" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="N7" s="39" t="s">
+      <c r="N7" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O7" s="66" t="s">
+      <c r="O7" s="65" t="s">
         <v>308</v>
       </c>
-      <c r="P7" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="39">
+      <c r="P7" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="38">
         <f t="shared" si="0"/>
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="R7" s="39" t="s">
+      <c r="R7" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V7">
@@ -5375,56 +5400,55 @@
       <c r="A8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="38">
         <v>3</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="39">
-        <v>0</v>
-      </c>
-      <c r="G8" s="39" t="s">
+      <c r="F8" s="38">
+        <v>0</v>
+      </c>
+      <c r="G8" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="77">
-        <f>0.3/9960</f>
-        <v>3.0120481927710842E-5</v>
-      </c>
-      <c r="I8" s="39" t="s">
+      <c r="H8" s="76">
+        <v>4.473795180722892E-4</v>
+      </c>
+      <c r="I8" s="38" t="s">
         <v>312</v>
       </c>
-      <c r="J8" s="39">
-        <v>0</v>
-      </c>
-      <c r="K8" s="41">
-        <v>0</v>
-      </c>
-      <c r="L8" s="39">
-        <v>0</v>
-      </c>
-      <c r="M8" s="39" t="s">
+      <c r="J8" s="38">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0</v>
+      </c>
+      <c r="L8" s="38">
+        <v>0</v>
+      </c>
+      <c r="M8" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="N8" s="39" t="s">
+      <c r="N8" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O8" s="67" t="s">
+      <c r="O8" s="66" t="s">
         <v>297</v>
       </c>
-      <c r="P8" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="75">
+      <c r="P8" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="74">
         <v>0.113</v>
       </c>
-      <c r="R8" s="39" t="s">
+      <c r="R8" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V8">
@@ -5438,55 +5462,55 @@
       <c r="A9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="38">
         <v>5</v>
       </c>
-      <c r="C9" s="39" t="s">
+      <c r="C9" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="39" t="s">
+      <c r="D9" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="E9" s="39" t="s">
+      <c r="E9" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="39">
-        <v>0</v>
-      </c>
-      <c r="G9" s="39">
-        <v>0</v>
-      </c>
-      <c r="H9" s="39">
-        <v>0</v>
-      </c>
-      <c r="I9" s="39" t="s">
+      <c r="F9" s="38">
+        <v>0</v>
+      </c>
+      <c r="G9" s="38">
+        <v>0</v>
+      </c>
+      <c r="H9" s="38">
+        <v>0</v>
+      </c>
+      <c r="I9" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J9" s="39">
-        <v>0</v>
-      </c>
-      <c r="K9" s="41">
-        <v>0</v>
-      </c>
-      <c r="L9" s="39">
-        <v>0</v>
-      </c>
-      <c r="M9" s="39" t="s">
+      <c r="J9" s="38">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
+      </c>
+      <c r="L9" s="38">
+        <v>0</v>
+      </c>
+      <c r="M9" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O9" s="68" t="s">
+      <c r="O9" s="67" t="s">
         <v>265</v>
       </c>
-      <c r="P9" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="45" t="s">
+      <c r="P9" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="R9" s="39" t="s">
+      <c r="R9" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V9" t="s">
@@ -5500,55 +5524,55 @@
       <c r="A10" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="39">
+      <c r="B10" s="38">
         <v>6</v>
       </c>
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="39">
-        <v>0</v>
-      </c>
-      <c r="G10" s="39">
-        <v>0</v>
-      </c>
-      <c r="H10" s="39">
-        <v>0</v>
-      </c>
-      <c r="I10" s="39" t="s">
+      <c r="F10" s="38">
+        <v>0</v>
+      </c>
+      <c r="G10" s="38">
+        <v>0</v>
+      </c>
+      <c r="H10" s="38">
+        <v>0</v>
+      </c>
+      <c r="I10" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="J10" s="39">
-        <v>0</v>
-      </c>
-      <c r="K10" s="41">
-        <v>0</v>
-      </c>
-      <c r="L10" s="39">
-        <v>0</v>
-      </c>
-      <c r="M10" s="39" t="s">
+      <c r="J10" s="38">
+        <v>0</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
+      </c>
+      <c r="L10" s="38">
+        <v>0</v>
+      </c>
+      <c r="M10" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="N10" s="39" t="s">
+      <c r="N10" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O10" s="68" t="s">
+      <c r="O10" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="P10" s="39">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="45" t="s">
+      <c r="P10" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="44" t="s">
         <v>229</v>
       </c>
-      <c r="R10" s="39" t="s">
+      <c r="R10" s="38" t="s">
         <v>309</v>
       </c>
       <c r="V10">
@@ -5593,31 +5617,31 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="62" t="s">
+      <c r="H1" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="62" t="s">
+      <c r="I1" s="61" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="62" t="s">
         <v>63</v>
       </c>
       <c r="K1" s="13" t="s">
@@ -5631,37 +5655,37 @@
       <c r="A2" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="52">
-        <v>0</v>
-      </c>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="51">
+        <v>0</v>
+      </c>
+      <c r="C2" s="52" t="s">
         <v>60</v>
       </c>
       <c r="D2">
         <v>0.2</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="54">
+      <c r="F2" s="53">
         <v>0.129</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="36">
-        <v>0</v>
-      </c>
-      <c r="I2" s="36">
-        <v>0</v>
-      </c>
-      <c r="J2" s="36">
-        <v>0</v>
-      </c>
-      <c r="K2" s="36" t="s">
+      <c r="H2" s="35">
+        <v>0</v>
+      </c>
+      <c r="I2" s="35">
+        <v>0</v>
+      </c>
+      <c r="J2" s="35">
+        <v>0</v>
+      </c>
+      <c r="K2" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="L2" s="76" t="s">
+      <c r="L2" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5669,22 +5693,22 @@
       <c r="A3" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="55">
-        <v>0</v>
-      </c>
-      <c r="C3" s="56" t="s">
+      <c r="B3" s="54">
+        <v>0</v>
+      </c>
+      <c r="C3" s="55" t="s">
         <v>60</v>
       </c>
       <c r="D3">
         <v>0.2</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="57">
+      <c r="F3" s="56">
         <v>0.129</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="55" t="s">
         <v>60</v>
       </c>
       <c r="H3">
@@ -5699,7 +5723,7 @@
       <c r="K3" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5707,22 +5731,22 @@
       <c r="A4" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="B4" s="55">
-        <v>0</v>
-      </c>
-      <c r="C4" s="56" t="s">
+      <c r="B4" s="54">
+        <v>0</v>
+      </c>
+      <c r="C4" s="55" t="s">
         <v>60</v>
       </c>
       <c r="D4">
         <v>0.2</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="57">
+      <c r="F4" s="56">
         <v>0.129</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="55" t="s">
         <v>60</v>
       </c>
       <c r="H4">
@@ -5737,7 +5761,7 @@
       <c r="K4" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="76" t="s">
+      <c r="L4" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5745,22 +5769,22 @@
       <c r="A5" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B5" s="55">
-        <v>0</v>
-      </c>
-      <c r="C5" s="56" t="s">
+      <c r="B5" s="54">
+        <v>0</v>
+      </c>
+      <c r="C5" s="55" t="s">
         <v>60</v>
       </c>
       <c r="D5">
         <v>0.2</v>
       </c>
-      <c r="E5" s="56" t="s">
+      <c r="E5" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="57">
+      <c r="F5" s="56">
         <v>0.129</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="55" t="s">
         <v>60</v>
       </c>
       <c r="H5">
@@ -5775,7 +5799,7 @@
       <c r="K5" t="s">
         <v>64</v>
       </c>
-      <c r="L5" s="76" t="s">
+      <c r="L5" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5783,22 +5807,22 @@
       <c r="A6" s="16" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="55">
-        <v>0</v>
-      </c>
-      <c r="C6" s="56" t="s">
+      <c r="B6" s="54">
+        <v>0</v>
+      </c>
+      <c r="C6" s="55" t="s">
         <v>60</v>
       </c>
       <c r="D6">
         <v>0.2</v>
       </c>
-      <c r="E6" s="56" t="s">
+      <c r="E6" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F6" s="57">
+      <c r="F6" s="56">
         <v>0.129</v>
       </c>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="55" t="s">
         <v>60</v>
       </c>
       <c r="H6">
@@ -5813,7 +5837,7 @@
       <c r="K6" t="s">
         <v>64</v>
       </c>
-      <c r="L6" s="76" t="s">
+      <c r="L6" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5821,37 +5845,37 @@
       <c r="A7" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="58">
-        <v>0</v>
-      </c>
-      <c r="C7" s="59" t="s">
+      <c r="B7" s="57">
+        <v>0</v>
+      </c>
+      <c r="C7" s="58" t="s">
         <v>60</v>
       </c>
       <c r="D7">
         <v>0.2</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="F7" s="61">
+      <c r="F7" s="60">
         <v>0.129</v>
       </c>
-      <c r="G7" s="59" t="s">
+      <c r="G7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="60">
-        <v>0</v>
-      </c>
-      <c r="I7" s="60">
-        <v>0</v>
-      </c>
-      <c r="J7" s="60">
-        <v>0</v>
-      </c>
-      <c r="K7" s="60" t="s">
+      <c r="H7" s="59">
+        <v>0</v>
+      </c>
+      <c r="I7" s="59">
+        <v>0</v>
+      </c>
+      <c r="J7" s="59">
+        <v>0</v>
+      </c>
+      <c r="K7" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="L7" s="76" t="s">
+      <c r="L7" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5859,37 +5883,37 @@
       <c r="A8" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="51">
         <v>45</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="52" t="s">
         <v>60</v>
       </c>
       <c r="D8">
         <v>0.2</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="54">
+      <c r="F8" s="53">
         <v>1.27E-4</v>
       </c>
-      <c r="G8" s="53" t="s">
+      <c r="G8" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="36">
-        <v>0</v>
-      </c>
-      <c r="I8" s="36">
-        <v>0</v>
-      </c>
-      <c r="J8" s="36">
-        <v>0</v>
-      </c>
-      <c r="K8" s="36" t="s">
+      <c r="H8" s="35">
+        <v>0</v>
+      </c>
+      <c r="I8" s="35">
+        <v>0</v>
+      </c>
+      <c r="J8" s="35">
+        <v>0</v>
+      </c>
+      <c r="K8" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="L8" s="76" t="s">
+      <c r="L8" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5897,22 +5921,22 @@
       <c r="A9" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B9" s="55">
-        <v>0</v>
-      </c>
-      <c r="C9" s="56" t="s">
+      <c r="B9" s="54">
+        <v>0</v>
+      </c>
+      <c r="C9" s="55" t="s">
         <v>60</v>
       </c>
       <c r="D9">
         <v>0.2</v>
       </c>
-      <c r="E9" s="56" t="s">
+      <c r="E9" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="57">
+      <c r="F9" s="56">
         <v>1.27E-4</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="55" t="s">
         <v>60</v>
       </c>
       <c r="H9">
@@ -5927,7 +5951,7 @@
       <c r="K9" t="s">
         <v>64</v>
       </c>
-      <c r="L9" s="76" t="s">
+      <c r="L9" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5935,37 +5959,37 @@
       <c r="A10" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B10" s="58">
-        <v>0</v>
-      </c>
-      <c r="C10" s="59" t="s">
+      <c r="B10" s="57">
+        <v>0</v>
+      </c>
+      <c r="C10" s="58" t="s">
         <v>60</v>
       </c>
       <c r="D10">
         <v>0.2</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="F10" s="61">
+      <c r="F10" s="60">
         <v>1.27E-4</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="H10" s="60">
-        <v>0</v>
-      </c>
-      <c r="I10" s="60">
-        <v>0</v>
-      </c>
-      <c r="J10" s="60">
-        <v>0</v>
-      </c>
-      <c r="K10" s="60" t="s">
+      <c r="H10" s="59">
+        <v>0</v>
+      </c>
+      <c r="I10" s="59">
+        <v>0</v>
+      </c>
+      <c r="J10" s="59">
+        <v>0</v>
+      </c>
+      <c r="K10" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="L10" s="76" t="s">
+      <c r="L10" s="75" t="s">
         <v>310</v>
       </c>
     </row>
@@ -6005,22 +6029,22 @@
       <c r="B1" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>45</v>
       </c>
       <c r="I1" s="16" t="s">
@@ -6043,7 +6067,7 @@
       </c>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="29" t="s">
         <v>194</v>
       </c>
       <c r="B2" s="12">
@@ -6087,7 +6111,7 @@
       </c>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>104</v>
       </c>
       <c r="B3" s="9">
@@ -6131,7 +6155,7 @@
       </c>
     </row>
     <row r="4" spans="1:14">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>105</v>
       </c>
       <c r="B4" s="9">
@@ -6175,7 +6199,7 @@
       </c>
     </row>
     <row r="5" spans="1:14">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="28" t="s">
         <v>106</v>
       </c>
       <c r="B5" s="9">
@@ -6205,7 +6229,7 @@
       <c r="J5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="30">
         <v>0</v>
       </c>
       <c r="L5" s="9">
@@ -6219,7 +6243,7 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>107</v>
       </c>
       <c r="B6" s="9">
@@ -6263,7 +6287,7 @@
       </c>
     </row>
     <row r="7" spans="1:14">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>108</v>
       </c>
       <c r="B7" s="9">
@@ -6307,7 +6331,7 @@
       </c>
     </row>
     <row r="8" spans="1:14">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>45</v>
       </c>
       <c r="B8" s="9">
@@ -6625,7 +6649,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D4 C3 E5 F6 G7 H8">
+  <conditionalFormatting sqref="C3 D4 E5 F6 G7 H8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6696,19 +6720,19 @@
       <c r="A2" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C2" s="28">
-        <v>0</v>
-      </c>
-      <c r="D2" s="28">
-        <v>0</v>
-      </c>
-      <c r="E2" s="28">
-        <v>0</v>
-      </c>
-      <c r="F2" s="28">
+      <c r="C2" s="27">
+        <v>0</v>
+      </c>
+      <c r="D2" s="27">
+        <v>0</v>
+      </c>
+      <c r="E2" s="27">
+        <v>0</v>
+      </c>
+      <c r="F2" s="27">
         <v>0</v>
       </c>
       <c r="G2" s="11" t="s">
@@ -6725,19 +6749,19 @@
       <c r="A3" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="28">
-        <v>0</v>
-      </c>
-      <c r="D3" s="28">
-        <v>0</v>
-      </c>
-      <c r="E3" s="28">
-        <v>0</v>
-      </c>
-      <c r="F3" s="28">
+      <c r="C3" s="27">
+        <v>0</v>
+      </c>
+      <c r="D3" s="27">
+        <v>0</v>
+      </c>
+      <c r="E3" s="27">
+        <v>0</v>
+      </c>
+      <c r="F3" s="27">
         <v>0</v>
       </c>
       <c r="G3" s="11" t="s">
@@ -6754,19 +6778,19 @@
       <c r="A4" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C4" s="28">
-        <v>0</v>
-      </c>
-      <c r="D4" s="28">
-        <v>0</v>
-      </c>
-      <c r="E4" s="28">
-        <v>0</v>
-      </c>
-      <c r="F4" s="28">
+      <c r="C4" s="27">
+        <v>0</v>
+      </c>
+      <c r="D4" s="27">
+        <v>0</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0</v>
+      </c>
+      <c r="F4" s="27">
         <v>0</v>
       </c>
       <c r="G4" s="11" t="s">
@@ -6783,19 +6807,19 @@
       <c r="A5" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C5" s="28">
-        <v>0</v>
-      </c>
-      <c r="D5" s="28">
-        <v>0</v>
-      </c>
-      <c r="E5" s="28">
-        <v>0</v>
-      </c>
-      <c r="F5" s="28">
+      <c r="C5" s="27">
+        <v>0</v>
+      </c>
+      <c r="D5" s="27">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0</v>
+      </c>
+      <c r="F5" s="27">
         <v>0</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -6812,19 +6836,19 @@
       <c r="A6" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C6" s="28">
-        <v>0</v>
-      </c>
-      <c r="D6" s="28">
-        <v>0</v>
-      </c>
-      <c r="E6" s="28">
-        <v>0</v>
-      </c>
-      <c r="F6" s="28">
+      <c r="C6" s="27">
+        <v>0</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27">
         <v>0</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -6841,41 +6865,41 @@
       <c r="A7" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B7" s="28">
-        <v>0</v>
-      </c>
-      <c r="C7" s="34">
-        <v>0</v>
-      </c>
-      <c r="D7" s="34" t="s">
+      <c r="B7" s="27">
+        <v>0</v>
+      </c>
+      <c r="C7" s="33">
+        <v>0</v>
+      </c>
+      <c r="D7" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="33" t="s">
         <v>197</v>
       </c>
-      <c r="F7" s="34" t="s">
+      <c r="F7" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="G7" s="35">
+      <c r="G7" s="34">
         <v>0</v>
       </c>
       <c r="H7" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="34" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="21"/>
       <c r="B8" s="4"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
     </row>
     <row r="9" spans="1:9">
       <c r="H9" s="25"/>
@@ -7105,10 +7129,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>37</v>
       </c>
     </row>
@@ -7381,10 +7405,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE819A9C-4E64-4D0F-8F31-2F1BF4DCFD79}">
-  <dimension ref="A1:Z36"/>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y20" sqref="Y20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7403,9 +7427,10 @@
     <col min="18" max="18" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.54296875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>81</v>
       </c>
@@ -7413,15 +7438,15 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
-      <c r="P2" s="69" t="s">
+    <row r="2" spans="1:27">
+      <c r="P2" s="68" t="s">
         <v>257</v>
       </c>
-      <c r="X2" s="69" t="s">
+      <c r="X2" s="68" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:27">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -7472,7 +7497,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:27">
       <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
@@ -7488,13 +7513,13 @@
       <c r="E4" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G4" s="72" t="s">
+      <c r="G4" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H4" s="73" t="s">
+      <c r="H4" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I4" s="51" t="s">
+      <c r="I4" s="50" t="s">
         <v>255</v>
       </c>
       <c r="K4">
@@ -7518,13 +7543,13 @@
       <c r="R4" t="s">
         <v>259</v>
       </c>
-      <c r="S4" s="37" t="s">
+      <c r="S4" s="36" t="s">
         <v>256</v>
       </c>
       <c r="X4" t="s">
         <v>301</v>
       </c>
-      <c r="Y4" s="57">
+      <c r="Y4" s="56">
         <f>(0.5 +0.17 +0.38+0.08) *1000</f>
         <v>1130.0000000000002</v>
       </c>
@@ -7532,7 +7557,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:27">
       <c r="A5" s="16" t="s">
         <v>7</v>
       </c>
@@ -7548,13 +7573,13 @@
       <c r="E5" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G5" s="72" t="s">
+      <c r="G5" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H5" s="73" t="s">
+      <c r="H5" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="I5" s="50" t="s">
         <v>255</v>
       </c>
       <c r="K5">
@@ -7578,7 +7603,7 @@
       <c r="R5" t="s">
         <v>260</v>
       </c>
-      <c r="S5" s="37" t="s">
+      <c r="S5" s="36" t="s">
         <v>262</v>
       </c>
       <c r="X5" t="s">
@@ -7591,7 +7616,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:27">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -7607,13 +7632,13 @@
       <c r="E6" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G6" s="72" t="s">
+      <c r="G6" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H6" s="73" t="s">
+      <c r="H6" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I6" s="51" t="s">
+      <c r="I6" s="50" t="s">
         <v>255</v>
       </c>
       <c r="K6">
@@ -7638,7 +7663,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15" thickBot="1">
+    <row r="7" spans="1:27" ht="15" thickBot="1">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
@@ -7654,17 +7679,17 @@
       <c r="E7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G7" s="72" t="s">
+      <c r="G7" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H7" s="73" t="s">
+      <c r="H7" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I7" s="51" t="s">
+      <c r="I7" s="50" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" thickBot="1">
+    <row r="8" spans="1:27" ht="15" thickBot="1">
       <c r="A8" s="16" t="s">
         <v>25</v>
       </c>
@@ -7680,35 +7705,35 @@
       <c r="E8" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="G8" s="72" t="s">
+      <c r="G8" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H8" s="73" t="s">
+      <c r="H8" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I8" s="51" t="s">
+      <c r="I8" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="K8" s="48" t="s">
+      <c r="K8" s="47" t="s">
         <v>253</v>
       </c>
-      <c r="L8" s="49">
+      <c r="L8" s="48">
         <f>AVERAGE(K4:K6)</f>
         <v>42.373333333333335</v>
       </c>
-      <c r="M8" s="50" t="s">
+      <c r="M8" s="49" t="s">
         <v>254</v>
       </c>
-      <c r="P8" s="69" t="s">
+      <c r="P8" s="68" t="s">
         <v>266</v>
       </c>
-      <c r="R8" s="37" t="s">
+      <c r="R8" s="36" t="s">
         <v>281</v>
       </c>
       <c r="X8" t="s">
         <v>302</v>
       </c>
-      <c r="Y8" s="71">
+      <c r="Y8" s="70">
         <f xml:space="preserve"> Y4/(Y5 )</f>
         <v>0.1134538152610442</v>
       </c>
@@ -7716,7 +7741,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="9" spans="1:26">
+    <row r="9" spans="1:27">
       <c r="A9" s="16" t="s">
         <v>45</v>
       </c>
@@ -7732,13 +7757,13 @@
       <c r="E9" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G9" s="72" t="s">
+      <c r="G9" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H9" s="73" t="s">
+      <c r="H9" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I9" s="51" t="s">
+      <c r="I9" s="50" t="s">
         <v>255</v>
       </c>
       <c r="P9" s="1" t="s">
@@ -7754,7 +7779,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:26">
+    <row r="10" spans="1:27">
       <c r="A10" s="15" t="s">
         <v>53</v>
       </c>
@@ -7764,7 +7789,7 @@
       <c r="C10" t="s">
         <v>169</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="72" t="s">
         <v>169</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -7773,10 +7798,10 @@
       <c r="G10" s="20" t="s">
         <v>285</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I10" s="74" t="s">
+      <c r="I10" s="73" t="s">
         <v>287</v>
       </c>
       <c r="P10" t="s">
@@ -7792,7 +7817,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="11" spans="1:26">
+    <row r="11" spans="1:27">
       <c r="A11" s="15" t="s">
         <v>264</v>
       </c>
@@ -7808,26 +7833,26 @@
       <c r="E11" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G11" s="72" t="s">
+      <c r="G11" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H11" s="73" t="s">
+      <c r="H11" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I11" s="74" t="s">
+      <c r="I11" s="73" t="s">
         <v>287</v>
       </c>
       <c r="P11" t="s">
         <v>272</v>
       </c>
-      <c r="Q11" s="70">
+      <c r="Q11" s="69">
         <v>2.83</v>
       </c>
       <c r="R11" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:27">
       <c r="A12" s="15" t="s">
         <v>50</v>
       </c>
@@ -7843,13 +7868,13 @@
       <c r="E12" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G12" s="72" t="s">
+      <c r="G12" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H12" s="73" t="s">
+      <c r="H12" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I12" s="74" t="s">
+      <c r="I12" s="73" t="s">
         <v>262</v>
       </c>
       <c r="P12" t="s">
@@ -7861,12 +7886,15 @@
       <c r="R12" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="13" spans="1:26">
+      <c r="X12" s="68" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="26" t="s">
         <v>175</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -7878,13 +7906,13 @@
       <c r="E13" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G13" s="72" t="s">
+      <c r="G13" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I13" s="74" t="s">
+      <c r="I13" s="73" t="s">
         <v>262</v>
       </c>
       <c r="P13" t="s">
@@ -7896,12 +7924,24 @@
       <c r="R13" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="14" spans="1:26">
+      <c r="X13" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="26" t="s">
         <v>175</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -7913,30 +7953,51 @@
       <c r="E14" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="G14" s="72" t="s">
+      <c r="G14" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="H14" s="73" t="s">
+      <c r="H14" s="72" t="s">
         <v>286</v>
       </c>
-      <c r="I14" s="74" t="s">
+      <c r="I14" s="73" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="15" spans="1:26">
+      <c r="X14" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y14">
+        <v>9960</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="C15" s="4"/>
       <c r="P15" t="s">
         <v>279</v>
       </c>
-      <c r="Q15" s="70">
+      <c r="Q15" s="69">
         <f>Q11*Q12*Q13</f>
         <v>32.262</v>
       </c>
       <c r="R15" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="16" spans="1:26">
+      <c r="X15" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y15">
+        <v>9902</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>278</v>
+      </c>
+      <c r="AA15" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="C16" s="4"/>
       <c r="P16" t="s">
         <v>280</v>
@@ -7945,17 +8006,60 @@
         <f>Q15/Q10</f>
         <v>8.0655000000000004E-2</v>
       </c>
-    </row>
-    <row r="17" spans="16:18">
-      <c r="Q17" s="70">
+      <c r="X16" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y16">
+        <v>0.45</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA16" s="36" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="17" spans="16:26">
+      <c r="Q17" s="69">
         <f>Q16*100</f>
         <v>8.0655000000000001</v>
       </c>
       <c r="R17" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="26" spans="16:18">
+      <c r="X17" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y17">
+        <f xml:space="preserve"> Y15*Y16</f>
+        <v>4455.9000000000005</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="18" spans="16:26">
+      <c r="Y18">
+        <f>Y17*10^(-3)</f>
+        <v>4.4559000000000006</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="16:26">
+      <c r="X20" t="s">
+        <v>318</v>
+      </c>
+      <c r="Y20" s="56">
+        <f>Y18/Y14</f>
+        <v>4.473795180722892E-4</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" spans="16:26">
       <c r="P26" t="s">
         <v>271</v>
       </c>
@@ -7966,7 +8070,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="27" spans="16:18">
+    <row r="27" spans="16:26">
       <c r="P27" t="s">
         <v>271</v>
       </c>
@@ -7978,7 +8082,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="29" spans="16:18">
+    <row r="29" spans="16:26">
       <c r="P29" t="s">
         <v>274</v>
       </c>
@@ -7989,7 +8093,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="16:18">
+    <row r="30" spans="16:26">
       <c r="P30" t="s">
         <v>274</v>
       </c>
@@ -8001,7 +8105,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="32" spans="16:18">
+    <row r="32" spans="16:26">
       <c r="P32" t="s">
         <v>290</v>
       </c>
@@ -8061,9 +8165,11 @@
     <hyperlink ref="I8" r:id="rId14" xr:uid="{778974ED-15CC-4E14-B7D5-9C50F3C9F709}"/>
     <hyperlink ref="I7" r:id="rId15" xr:uid="{F4A4DDC8-517D-4A51-B6F8-22DB8A85D725}"/>
     <hyperlink ref="I9" r:id="rId16" xr:uid="{DE7EA573-101C-4361-90D7-A078870E63AD}"/>
+    <hyperlink ref="D10" r:id="rId17" xr:uid="{22AD580D-B18A-4955-B323-32557020E021}"/>
+    <hyperlink ref="AA15" r:id="rId18" xr:uid="{9D2F1804-135A-4DD9-ABDD-9617C04DA008}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId17"/>
-  <drawing r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId19"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Making version1 and version2 case studies
</commit_message>
<xml_diff>
--- a/excel files/propionate_case_study_v2.xlsx
+++ b/excel files/propionate_case_study_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C203BE-6357-4C1F-85F6-BCD6B0E593A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60D8595-DCC4-47D6-A639-6A984425B54C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="319">
   <si>
     <t>components</t>
   </si>
@@ -602,21 +602,6 @@
     <t>select</t>
   </si>
   <si>
-    <t>PAC_v2.json</t>
-  </si>
-  <si>
-    <t>sherm_v2.json</t>
-  </si>
-  <si>
-    <t>avidum_v2.json</t>
-  </si>
-  <si>
-    <t>acnes_v2.json</t>
-  </si>
-  <si>
-    <t>propionicum_v2.json</t>
-  </si>
-  <si>
     <t>Maltose</t>
   </si>
   <si>
@@ -752,12 +737,6 @@
     <t>fed-batch (FFB, biomass contained in fibers)</t>
   </si>
   <si>
-    <t>Distillation_2.json</t>
-  </si>
-  <si>
-    <t>Distillation_3.json</t>
-  </si>
-  <si>
     <t>https://shuowanchemical.en.made-in-china.com/product/XQoUxvSJhVcb/China-99-5-CAS-79-09-4-Propionic-Acid-for-Food-Preservatives.html</t>
   </si>
   <si>
@@ -1029,6 +1008,21 @@
   </si>
   <si>
     <t>g/h</t>
+  </si>
+  <si>
+    <t>v2_PAC.json</t>
+  </si>
+  <si>
+    <t>v2_sherm.json</t>
+  </si>
+  <si>
+    <t>v2_avidum.json</t>
+  </si>
+  <si>
+    <t>v2_acnes.json</t>
+  </si>
+  <si>
+    <t>v2_propionicum.json</t>
   </si>
 </sst>
 </file>
@@ -4151,7 +4145,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:H4"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
@@ -4206,7 +4200,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C2" s="4">
         <v>1000</v>
@@ -4215,10 +4209,10 @@
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G2" s="4">
         <v>0</v>
@@ -4227,7 +4221,7 @@
         <v>60</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="J2" s="4">
         <v>1</v>
@@ -4247,7 +4241,7 @@
         <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F3" s="4">
         <v>0</v>
@@ -4279,7 +4273,7 @@
         <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -4334,13 +4328,13 @@
         <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E1" t="s">
         <v>120</v>
@@ -4351,13 +4345,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="25" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B2">
         <v>0.37</v>
       </c>
       <c r="C2" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D2" s="69">
         <f>B2*1/1.1</f>
@@ -4367,18 +4361,18 @@
         <v>60</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="77" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B3">
         <v>1.85</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D3" s="69">
         <f t="shared" ref="D3:D12" si="0">B3*1/1.1</f>
@@ -4388,18 +4382,18 @@
         <v>60</v>
       </c>
       <c r="F3" s="36" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="25" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B4">
         <v>0.4</v>
       </c>
       <c r="C4" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D4" s="69">
         <f t="shared" si="0"/>
@@ -4409,18 +4403,18 @@
         <v>60</v>
       </c>
       <c r="F4" s="36" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B5">
         <v>0.51</v>
       </c>
       <c r="C5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D5" s="69">
         <f t="shared" si="0"/>
@@ -4430,18 +4424,18 @@
         <v>60</v>
       </c>
       <c r="F5" s="36" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="25" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D6" s="69">
         <f t="shared" si="0"/>
@@ -4451,18 +4445,18 @@
         <v>60</v>
       </c>
       <c r="F6" s="36" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="77" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D7" s="69">
         <f t="shared" si="0"/>
@@ -4472,18 +4466,18 @@
         <v>60</v>
       </c>
       <c r="F7" s="36" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="25" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B8">
         <v>3.5</v>
       </c>
       <c r="C8" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D8" s="69">
         <f t="shared" si="0"/>
@@ -4493,18 +4487,18 @@
         <v>60</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="25" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B9">
         <v>0.85</v>
       </c>
       <c r="C9" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D9" s="69">
         <f t="shared" si="0"/>
@@ -4514,18 +4508,18 @@
         <v>60</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="25" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B10">
         <v>0.45</v>
       </c>
       <c r="C10" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D10" s="69">
         <f t="shared" si="0"/>
@@ -4535,19 +4529,19 @@
         <v>60</v>
       </c>
       <c r="F10" s="36" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="45" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B11">
         <f>2.25 *1.1</f>
         <v>2.4750000000000001</v>
       </c>
       <c r="C11" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D11" s="69">
         <f t="shared" si="0"/>
@@ -4557,19 +4551,19 @@
         <v>60</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="45" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B12">
         <f>0.6*1.1</f>
         <v>0.66</v>
       </c>
       <c r="C12" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D12" s="69">
         <f t="shared" si="0"/>
@@ -4579,7 +4573,7 @@
         <v>60</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -4627,7 +4621,7 @@
         <v>85</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
@@ -4638,7 +4632,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="25" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B2">
         <v>222</v>
@@ -4647,12 +4641,12 @@
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="25" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B3">
         <v>85.8</v>
@@ -4661,12 +4655,12 @@
         <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="25" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B4">
         <v>64.3</v>
@@ -4675,12 +4669,12 @@
         <v>60</v>
       </c>
       <c r="D4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="25" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B5">
         <v>74.8</v>
@@ -4689,12 +4683,12 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="25" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>61.1</v>
@@ -4703,12 +4697,12 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="25" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B7">
         <v>381</v>
@@ -4717,12 +4711,12 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="25" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B8">
         <v>53.6</v>
@@ -4731,12 +4725,12 @@
         <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="25" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B9">
         <v>53.3</v>
@@ -4745,12 +4739,12 @@
         <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="25" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B10">
         <v>52.3</v>
@@ -4759,12 +4753,12 @@
         <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="25" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B11">
         <v>78.5</v>
@@ -4773,15 +4767,15 @@
         <v>60</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E11" s="37" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="25" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B12">
         <v>50.5</v>
@@ -4790,10 +4784,10 @@
         <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E12" s="37" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -4823,27 +4817,27 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
         <v>59</v>
       </c>
       <c r="D1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" t="s">
         <v>220</v>
-      </c>
-      <c r="F1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="B2" s="4">
         <v>37</v>
@@ -4852,21 +4846,21 @@
         <v>67</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="E2" s="43" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F2" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
         <v>67</v>
@@ -4874,31 +4868,31 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B7" s="4">
         <v>71</v>
@@ -4907,10 +4901,10 @@
         <v>67</v>
       </c>
       <c r="D7" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="F7" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4926,8 +4920,8 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H13" sqref="H13"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4982,7 +4976,7 @@
         <v>66</v>
       </c>
       <c r="I1" s="41" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="J1" s="41" t="s">
         <v>109</v>
@@ -5029,7 +5023,7 @@
         <v>117</v>
       </c>
       <c r="D2" s="39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E2" s="38" t="s">
         <v>72</v>
@@ -5053,7 +5047,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="38" t="s">
-        <v>178</v>
+        <v>314</v>
       </c>
       <c r="M2" s="38" t="s">
         <v>99</v>
@@ -5062,7 +5056,7 @@
         <v>72</v>
       </c>
       <c r="O2" s="65" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="P2" s="38">
         <v>0</v>
@@ -5072,7 +5066,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R2" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -5092,7 +5086,7 @@
         <v>117</v>
       </c>
       <c r="D3" s="39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E3" s="38" t="s">
         <v>72</v>
@@ -5116,7 +5110,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>179</v>
+        <v>315</v>
       </c>
       <c r="M3" s="38" t="s">
         <v>99</v>
@@ -5125,7 +5119,7 @@
         <v>72</v>
       </c>
       <c r="O3" s="65" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="P3" s="38">
         <v>0</v>
@@ -5135,7 +5129,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R3" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V3">
         <v>0</v>
@@ -5155,7 +5149,7 @@
         <v>117</v>
       </c>
       <c r="D4" s="39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E4" s="38" t="s">
         <v>72</v>
@@ -5179,7 +5173,7 @@
         <v>0</v>
       </c>
       <c r="L4" s="38" t="s">
-        <v>180</v>
+        <v>316</v>
       </c>
       <c r="M4" s="38" t="s">
         <v>99</v>
@@ -5188,7 +5182,7 @@
         <v>72</v>
       </c>
       <c r="O4" s="65" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="P4" s="38">
         <v>0</v>
@@ -5198,7 +5192,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R4" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -5218,7 +5212,7 @@
         <v>117</v>
       </c>
       <c r="D5" s="39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E5" s="38" t="s">
         <v>72</v>
@@ -5242,7 +5236,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="38" t="s">
-        <v>181</v>
+        <v>317</v>
       </c>
       <c r="M5" s="38" t="s">
         <v>99</v>
@@ -5251,7 +5245,7 @@
         <v>72</v>
       </c>
       <c r="O5" s="65" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="P5" s="38">
         <v>0</v>
@@ -5261,7 +5255,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R5" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V5">
         <v>0</v>
@@ -5281,7 +5275,7 @@
         <v>117</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E6" s="38" t="s">
         <v>72</v>
@@ -5305,7 +5299,7 @@
         <v>0</v>
       </c>
       <c r="L6" s="38" t="s">
-        <v>182</v>
+        <v>318</v>
       </c>
       <c r="M6" s="38" t="s">
         <v>99</v>
@@ -5314,7 +5308,7 @@
         <v>72</v>
       </c>
       <c r="O6" s="65" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="P6" s="38">
         <v>0</v>
@@ -5324,7 +5318,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R6" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V6">
         <v>0</v>
@@ -5344,7 +5338,7 @@
         <v>117</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E7" s="38" t="s">
         <v>72</v>
@@ -5377,7 +5371,7 @@
         <v>72</v>
       </c>
       <c r="O7" s="65" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="P7" s="38">
         <v>0</v>
@@ -5387,7 +5381,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="R7" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -5422,7 +5416,7 @@
         <v>4.473795180722892E-4</v>
       </c>
       <c r="I8" s="38" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="J8" s="38">
         <v>0</v>
@@ -5440,7 +5434,7 @@
         <v>72</v>
       </c>
       <c r="O8" s="66" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="P8" s="38">
         <v>0</v>
@@ -5449,7 +5443,7 @@
         <v>0.113</v>
       </c>
       <c r="R8" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V8">
         <v>0</v>
@@ -5502,16 +5496,16 @@
         <v>72</v>
       </c>
       <c r="O9" s="67" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="P9" s="38">
         <v>0</v>
       </c>
-      <c r="Q9" s="44" t="s">
-        <v>228</v>
+      <c r="Q9" s="44">
+        <v>0.3</v>
       </c>
       <c r="R9" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V9" t="s">
         <v>79</v>
@@ -5569,11 +5563,11 @@
       <c r="P10" s="38">
         <v>0</v>
       </c>
-      <c r="Q10" s="44" t="s">
-        <v>229</v>
+      <c r="Q10" s="44">
+        <v>0.6</v>
       </c>
       <c r="R10" s="38" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="V10">
         <v>0</v>
@@ -5686,7 +5680,7 @@
         <v>64</v>
       </c>
       <c r="L2" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -5724,7 +5718,7 @@
         <v>64</v>
       </c>
       <c r="L3" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -5762,7 +5756,7 @@
         <v>64</v>
       </c>
       <c r="L4" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -5800,7 +5794,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -5838,7 +5832,7 @@
         <v>64</v>
       </c>
       <c r="L6" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -5876,7 +5870,7 @@
         <v>64</v>
       </c>
       <c r="L7" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -5914,7 +5908,7 @@
         <v>64</v>
       </c>
       <c r="L8" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -5952,7 +5946,7 @@
         <v>64</v>
       </c>
       <c r="L9" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -5990,7 +5984,7 @@
         <v>64</v>
       </c>
       <c r="L10" s="75" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -6027,7 +6021,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C1" s="28" t="s">
         <v>104</v>
@@ -6068,7 +6062,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="29" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="B2" s="12">
         <v>0</v>
@@ -6447,7 +6441,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>23</v>
@@ -6671,7 +6665,7 @@
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B18" sqref="B18"/>
+      <selection pane="topRight" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5"/>
@@ -6717,11 +6711,11 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="4" t="s">
-        <v>178</v>
+      <c r="A2" s="38" t="s">
+        <v>314</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C2" s="27">
         <v>0</v>
@@ -6746,11 +6740,11 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
-        <v>179</v>
+      <c r="A3" s="38" t="s">
+        <v>315</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C3" s="27">
         <v>0</v>
@@ -6775,11 +6769,11 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="4" t="s">
-        <v>180</v>
+      <c r="A4" s="38" t="s">
+        <v>316</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C4" s="27">
         <v>0</v>
@@ -6804,11 +6798,11 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="4" t="s">
-        <v>181</v>
+      <c r="A5" s="38" t="s">
+        <v>317</v>
       </c>
       <c r="B5" s="27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C5" s="27">
         <v>0</v>
@@ -6833,11 +6827,11 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="4" t="s">
-        <v>182</v>
+      <c r="A6" s="38" t="s">
+        <v>318</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="C6" s="27">
         <v>0</v>
@@ -6875,10 +6869,10 @@
         <v>46</v>
       </c>
       <c r="E7" s="33" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F7" s="33" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G7" s="34">
         <v>0</v>
@@ -7440,10 +7434,10 @@
     </row>
     <row r="2" spans="1:27">
       <c r="P2" s="68" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="X2" s="68" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:27">
@@ -7473,25 +7467,25 @@
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>57</v>
@@ -7517,44 +7511,44 @@
         <v>168</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I4" s="50" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="K4">
         <v>30</v>
       </c>
       <c r="L4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="M4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="N4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="P4">
         <v>0.129</v>
       </c>
       <c r="Q4" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="R4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="S4" s="36" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="X4" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="Y4" s="56">
         <f>(0.5 +0.17 +0.38+0.08) *1000</f>
         <v>1130.0000000000002</v>
       </c>
       <c r="Z4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:27">
@@ -7577,37 +7571,37 @@
         <v>168</v>
       </c>
       <c r="H5" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I5" s="50" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="K5">
         <v>52.5</v>
       </c>
       <c r="L5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="M5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="N5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="P5">
         <v>0.127</v>
       </c>
       <c r="Q5" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="R5" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="S5" s="36" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="X5" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="Y5">
         <v>9960</v>
@@ -7636,25 +7630,25 @@
         <v>168</v>
       </c>
       <c r="H6" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I6" s="50" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="K6">
         <v>44.62</v>
       </c>
       <c r="L6" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="M6" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="N6" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="X6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="Y6">
         <v>11363</v>
@@ -7683,10 +7677,10 @@
         <v>168</v>
       </c>
       <c r="H7" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I7" s="50" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="15" thickBot="1">
@@ -7709,36 +7703,36 @@
         <v>168</v>
       </c>
       <c r="H8" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I8" s="50" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="K8" s="47" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="L8" s="48">
         <f>AVERAGE(K4:K6)</f>
         <v>42.373333333333335</v>
       </c>
       <c r="M8" s="49" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="P8" s="68" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="R8" s="36" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="X8" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="Y8" s="70">
         <f xml:space="preserve"> Y4/(Y5 )</f>
         <v>0.1134538152610442</v>
       </c>
       <c r="Z8" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -7761,22 +7755,22 @@
         <v>168</v>
       </c>
       <c r="H9" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I9" s="50" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="X9" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -7796,39 +7790,39 @@
         <v>168</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H10" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I10" s="73" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="P10" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="Q10">
         <v>400</v>
       </c>
       <c r="R10" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="X10" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
     </row>
     <row r="11" spans="1:27">
       <c r="A11" s="15" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>168</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>168</v>
@@ -7837,19 +7831,19 @@
         <v>168</v>
       </c>
       <c r="H11" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I11" s="73" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="P11" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="Q11" s="69">
         <v>2.83</v>
       </c>
       <c r="R11" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -7872,22 +7866,22 @@
         <v>168</v>
       </c>
       <c r="H12" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I12" s="73" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="P12" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="Q12">
         <v>0.38</v>
       </c>
       <c r="R12" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="X12" s="68" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:27">
@@ -7910,28 +7904,28 @@
         <v>168</v>
       </c>
       <c r="H13" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I13" s="73" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="P13" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="Q13">
         <v>30</v>
       </c>
       <c r="R13" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>57</v>
@@ -7957,13 +7951,13 @@
         <v>168</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I14" s="73" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="X14" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="Y14">
         <v>9960</v>
@@ -7975,14 +7969,14 @@
     <row r="15" spans="1:27">
       <c r="C15" s="4"/>
       <c r="P15" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="Q15" s="69">
         <f>Q11*Q12*Q13</f>
         <v>32.262</v>
       </c>
       <c r="R15" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="X15" t="s">
         <v>93</v>
@@ -7991,7 +7985,7 @@
         <v>9902</v>
       </c>
       <c r="Z15" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="AA15" s="36" t="s">
         <v>169</v>
@@ -8000,14 +7994,14 @@
     <row r="16" spans="1:27">
       <c r="C16" s="4"/>
       <c r="P16" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="Q16">
         <f>Q15/Q10</f>
         <v>8.0655000000000004E-2</v>
       </c>
       <c r="X16" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="Y16">
         <v>0.45</v>
@@ -8016,7 +8010,7 @@
         <v>67</v>
       </c>
       <c r="AA16" s="36" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="16:26">
@@ -8025,17 +8019,17 @@
         <v>8.0655000000000001</v>
       </c>
       <c r="R17" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="X17" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="Y17">
         <f xml:space="preserve"> Y15*Y16</f>
         <v>4455.9000000000005</v>
       </c>
       <c r="Z17" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="16:26">
@@ -8049,101 +8043,101 @@
     </row>
     <row r="20" spans="16:26">
       <c r="X20" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="Y20" s="56">
         <f>Y18/Y14</f>
         <v>4.473795180722892E-4</v>
       </c>
       <c r="Z20" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="16:26">
       <c r="P26" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="Q26">
         <v>400</v>
       </c>
       <c r="R26" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="16:26">
       <c r="P27" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="Q27">
         <f>Q26/3600</f>
         <v>0.1111111111111111</v>
       </c>
       <c r="R27" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="29" spans="16:26">
       <c r="P29" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="Q29">
         <v>20</v>
       </c>
       <c r="R29" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
     </row>
     <row r="30" spans="16:26">
       <c r="P30" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="Q30">
         <f>Q29 *100</f>
         <v>2000</v>
       </c>
       <c r="R30" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="32" spans="16:26">
       <c r="P32" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="Q32">
         <f>Q30*Q27</f>
         <v>222.2222222222222</v>
       </c>
       <c r="R32" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="16:18">
       <c r="P33" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="Q33">
         <f>Q32</f>
         <v>222.2222222222222</v>
       </c>
       <c r="R33" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35" spans="16:18">
       <c r="P35" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="Q35">
         <f>Q33/Q26</f>
         <v>0.55555555555555547</v>
       </c>
       <c r="R35" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="16:18">
       <c r="P36" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>